<commit_message>
Add comprehensive German/Italian translations and UI improvements - Add i18n translation system with English, German, and Italian support - Translate home page, upload page, navigation, and dashboard components - Update header title to remove date - Set default chart selection to January 2026 - Ensure Upload Data menu item is always visible - Add role-based access control with password protection - Implement collapsible sidebar and filter panel with animations - Update sidebar to support light mode theme
</commit_message>
<xml_diff>
--- a/attachments/Inbound 411_PS4.XLSX
+++ b/attachments/Inbound 411_PS4.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9123" uniqueCount="2181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9543" uniqueCount="2233">
   <si>
     <t>180104337</t>
   </si>
@@ -6508,7 +6508,163 @@
     <t>168629297</t>
   </si>
   <si>
+    <t>180135724</t>
+  </si>
+  <si>
+    <t>4500031144</t>
+  </si>
+  <si>
+    <t>12299</t>
+  </si>
+  <si>
+    <t>180136240</t>
+  </si>
+  <si>
     <t>Not Started</t>
+  </si>
+  <si>
+    <t>180136393</t>
+  </si>
+  <si>
+    <t>4500032234</t>
+  </si>
+  <si>
+    <t>8001747-01</t>
+  </si>
+  <si>
+    <t>180136394</t>
+  </si>
+  <si>
+    <t>4500032233</t>
+  </si>
+  <si>
+    <t>168898925</t>
+  </si>
+  <si>
+    <t>180136618</t>
+  </si>
+  <si>
+    <t>5914967A</t>
+  </si>
+  <si>
+    <t>BUS BAR DC OUTPUT NO CAM LOCKS 900EX</t>
+  </si>
+  <si>
+    <t>4500031538</t>
+  </si>
+  <si>
+    <t>12333</t>
+  </si>
+  <si>
+    <t>180136620</t>
+  </si>
+  <si>
+    <t>5914951A</t>
+  </si>
+  <si>
+    <t>RAIL MTG COMP DIN35 1.38 IN LG PERF RoHS</t>
+  </si>
+  <si>
+    <t>5914952A</t>
+  </si>
+  <si>
+    <t>SLIDE PANEL POWER BRIDGE 900EX</t>
+  </si>
+  <si>
+    <t>180136646</t>
+  </si>
+  <si>
+    <t>4500029899</t>
+  </si>
+  <si>
+    <t>109203</t>
+  </si>
+  <si>
+    <t>180136948</t>
+  </si>
+  <si>
+    <t>4500032315</t>
+  </si>
+  <si>
+    <t>A2RW</t>
+  </si>
+  <si>
+    <t>180137124</t>
+  </si>
+  <si>
+    <t>1/5/2026</t>
+  </si>
+  <si>
+    <t>180137128</t>
+  </si>
+  <si>
+    <t>4500032362</t>
+  </si>
+  <si>
+    <t>1/5/2025</t>
+  </si>
+  <si>
+    <t>180137139</t>
+  </si>
+  <si>
+    <t>4500029767</t>
+  </si>
+  <si>
+    <t>180137140</t>
+  </si>
+  <si>
+    <t>180137141</t>
+  </si>
+  <si>
+    <t>180137142</t>
+  </si>
+  <si>
+    <t>180137199</t>
+  </si>
+  <si>
+    <t>6128234-02</t>
+  </si>
+  <si>
+    <t>180137200</t>
+  </si>
+  <si>
+    <t>6119021-02</t>
+  </si>
+  <si>
+    <t>180137201</t>
+  </si>
+  <si>
+    <t>6125118-01</t>
+  </si>
+  <si>
+    <t>180137202</t>
+  </si>
+  <si>
+    <t>374940</t>
+  </si>
+  <si>
+    <t>180137203</t>
+  </si>
+  <si>
+    <t>180137204</t>
+  </si>
+  <si>
+    <t>180137205</t>
+  </si>
+  <si>
+    <t>12220</t>
+  </si>
+  <si>
+    <t>180137206</t>
+  </si>
+  <si>
+    <t>12186</t>
+  </si>
+  <si>
+    <t>180137207</t>
+  </si>
+  <si>
+    <t>ACPF</t>
   </si>
   <si>
     <t>Document</t>
@@ -6658,7 +6814,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O760"/>
+  <dimension ref="A1:O795"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6685,49 +6841,49 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
-        <v>2166</v>
+        <v>2218</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2167</v>
+        <v>2219</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2168</v>
+        <v>2220</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2169</v>
+        <v>2221</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2170</v>
+        <v>2222</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>2171</v>
+        <v>2223</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>2172</v>
+        <v>2224</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>2173</v>
+        <v>2225</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>2174</v>
+        <v>2226</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>2175</v>
+        <v>2227</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>2176</v>
+        <v>2228</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>2177</v>
+        <v>2229</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>2178</v>
+        <v>2230</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>2179</v>
+        <v>2231</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>2180</v>
+        <v>2232</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -40894,12 +41050,1587 @@
         <v>45999</v>
       </c>
       <c r="M760" t="s">
+        <v>7</v>
+      </c>
+      <c r="N760" t="s">
+        <v>8</v>
+      </c>
+      <c r="O760" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="761" spans="1:15">
+      <c r="A761" t="s">
         <v>2165</v>
       </c>
-      <c r="N760" t="s">
-        <v>8</v>
-      </c>
-      <c r="O760" t="s">
+      <c r="B761" t="s">
+        <v>1</v>
+      </c>
+      <c r="C761" t="s">
+        <v>892</v>
+      </c>
+      <c r="D761" t="s">
+        <v>893</v>
+      </c>
+      <c r="E761" s="2">
+        <v>4</v>
+      </c>
+      <c r="F761" t="s">
+        <v>4</v>
+      </c>
+      <c r="G761" t="s">
+        <v>2166</v>
+      </c>
+      <c r="H761" t="s">
+        <v>1</v>
+      </c>
+      <c r="I761" t="s">
+        <v>2167</v>
+      </c>
+      <c r="J761" t="s">
+        <v>7</v>
+      </c>
+      <c r="K761" s="3"/>
+      <c r="L761" s="3">
+        <v>46001</v>
+      </c>
+      <c r="M761" t="s">
+        <v>7</v>
+      </c>
+      <c r="N761" t="s">
+        <v>8</v>
+      </c>
+      <c r="O761" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="762" spans="1:15">
+      <c r="A762" t="s">
+        <v>2165</v>
+      </c>
+      <c r="B762" t="s">
+        <v>53</v>
+      </c>
+      <c r="C762" t="s">
+        <v>991</v>
+      </c>
+      <c r="D762" t="s">
+        <v>992</v>
+      </c>
+      <c r="E762" s="2">
+        <v>4</v>
+      </c>
+      <c r="F762" t="s">
+        <v>4</v>
+      </c>
+      <c r="G762" t="s">
+        <v>2166</v>
+      </c>
+      <c r="H762" t="s">
+        <v>53</v>
+      </c>
+      <c r="I762" t="s">
+        <v>2167</v>
+      </c>
+      <c r="J762" t="s">
+        <v>7</v>
+      </c>
+      <c r="K762" s="3"/>
+      <c r="L762" s="3">
+        <v>46001</v>
+      </c>
+      <c r="M762" t="s">
+        <v>7</v>
+      </c>
+      <c r="N762" t="s">
+        <v>8</v>
+      </c>
+      <c r="O762" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="763" spans="1:15">
+      <c r="A763" t="s">
+        <v>2168</v>
+      </c>
+      <c r="B763" t="s">
+        <v>1</v>
+      </c>
+      <c r="C763" t="s">
+        <v>354</v>
+      </c>
+      <c r="D763" t="s">
+        <v>355</v>
+      </c>
+      <c r="E763" s="2">
+        <v>1000</v>
+      </c>
+      <c r="F763" t="s">
+        <v>4</v>
+      </c>
+      <c r="G763" t="s">
+        <v>2079</v>
+      </c>
+      <c r="H763" t="s">
+        <v>1</v>
+      </c>
+      <c r="I763" t="s">
+        <v>2080</v>
+      </c>
+      <c r="J763" t="s">
+        <v>7</v>
+      </c>
+      <c r="K763" s="3"/>
+      <c r="L763" s="3">
+        <v>46006</v>
+      </c>
+      <c r="M763" t="s">
+        <v>2169</v>
+      </c>
+      <c r="N763" t="s">
+        <v>8</v>
+      </c>
+      <c r="O763" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="764" spans="1:15">
+      <c r="A764" t="s">
+        <v>2170</v>
+      </c>
+      <c r="B764" t="s">
+        <v>1</v>
+      </c>
+      <c r="C764" t="s">
+        <v>379</v>
+      </c>
+      <c r="D764" t="s">
+        <v>380</v>
+      </c>
+      <c r="E764" s="2">
+        <v>100</v>
+      </c>
+      <c r="F764" t="s">
+        <v>4</v>
+      </c>
+      <c r="G764" t="s">
+        <v>2171</v>
+      </c>
+      <c r="H764" t="s">
+        <v>1</v>
+      </c>
+      <c r="I764" t="s">
+        <v>2172</v>
+      </c>
+      <c r="J764" t="s">
+        <v>7</v>
+      </c>
+      <c r="K764" s="3"/>
+      <c r="L764" s="3">
+        <v>46007</v>
+      </c>
+      <c r="M764" t="s">
+        <v>7</v>
+      </c>
+      <c r="N764" t="s">
+        <v>8</v>
+      </c>
+      <c r="O764" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="765" spans="1:15">
+      <c r="A765" t="s">
+        <v>2170</v>
+      </c>
+      <c r="B765" t="s">
+        <v>53</v>
+      </c>
+      <c r="C765" t="s">
+        <v>325</v>
+      </c>
+      <c r="D765" t="s">
+        <v>326</v>
+      </c>
+      <c r="E765" s="2">
+        <v>50</v>
+      </c>
+      <c r="F765" t="s">
+        <v>4</v>
+      </c>
+      <c r="G765" t="s">
+        <v>2171</v>
+      </c>
+      <c r="H765" t="s">
+        <v>53</v>
+      </c>
+      <c r="I765" t="s">
+        <v>2172</v>
+      </c>
+      <c r="J765" t="s">
+        <v>7</v>
+      </c>
+      <c r="K765" s="3"/>
+      <c r="L765" s="3">
+        <v>46007</v>
+      </c>
+      <c r="M765" t="s">
+        <v>7</v>
+      </c>
+      <c r="N765" t="s">
+        <v>8</v>
+      </c>
+      <c r="O765" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="766" spans="1:15">
+      <c r="A766" t="s">
+        <v>2170</v>
+      </c>
+      <c r="B766" t="s">
+        <v>21</v>
+      </c>
+      <c r="C766" t="s">
+        <v>177</v>
+      </c>
+      <c r="D766" t="s">
+        <v>178</v>
+      </c>
+      <c r="E766" s="2">
+        <v>1</v>
+      </c>
+      <c r="F766" t="s">
+        <v>4</v>
+      </c>
+      <c r="G766" t="s">
+        <v>2171</v>
+      </c>
+      <c r="H766" t="s">
+        <v>21</v>
+      </c>
+      <c r="I766" t="s">
+        <v>2172</v>
+      </c>
+      <c r="J766" t="s">
+        <v>7</v>
+      </c>
+      <c r="K766" s="3"/>
+      <c r="L766" s="3">
+        <v>46007</v>
+      </c>
+      <c r="M766" t="s">
+        <v>7</v>
+      </c>
+      <c r="N766" t="s">
+        <v>8</v>
+      </c>
+      <c r="O766" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="767" spans="1:15">
+      <c r="A767" t="s">
+        <v>2170</v>
+      </c>
+      <c r="B767" t="s">
+        <v>25</v>
+      </c>
+      <c r="C767" t="s">
+        <v>332</v>
+      </c>
+      <c r="D767" t="s">
+        <v>333</v>
+      </c>
+      <c r="E767" s="2">
+        <v>125</v>
+      </c>
+      <c r="F767" t="s">
+        <v>4</v>
+      </c>
+      <c r="G767" t="s">
+        <v>2171</v>
+      </c>
+      <c r="H767" t="s">
+        <v>25</v>
+      </c>
+      <c r="I767" t="s">
+        <v>2172</v>
+      </c>
+      <c r="J767" t="s">
+        <v>7</v>
+      </c>
+      <c r="K767" s="3"/>
+      <c r="L767" s="3">
+        <v>46007</v>
+      </c>
+      <c r="M767" t="s">
+        <v>7</v>
+      </c>
+      <c r="N767" t="s">
+        <v>8</v>
+      </c>
+      <c r="O767" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="768" spans="1:15">
+      <c r="A768" t="s">
+        <v>2173</v>
+      </c>
+      <c r="B768" t="s">
+        <v>1</v>
+      </c>
+      <c r="C768" t="s">
+        <v>2161</v>
+      </c>
+      <c r="D768" t="s">
+        <v>2162</v>
+      </c>
+      <c r="E768" s="2">
+        <v>6</v>
+      </c>
+      <c r="F768" t="s">
+        <v>4</v>
+      </c>
+      <c r="G768" t="s">
+        <v>2174</v>
+      </c>
+      <c r="H768" t="s">
+        <v>1</v>
+      </c>
+      <c r="I768" t="s">
+        <v>2175</v>
+      </c>
+      <c r="J768" t="s">
+        <v>7</v>
+      </c>
+      <c r="K768" s="3"/>
+      <c r="L768" s="3">
+        <v>46007</v>
+      </c>
+      <c r="M768" t="s">
+        <v>7</v>
+      </c>
+      <c r="N768" t="s">
+        <v>8</v>
+      </c>
+      <c r="O768" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="769" spans="1:15">
+      <c r="A769" t="s">
+        <v>2176</v>
+      </c>
+      <c r="B769" t="s">
+        <v>1</v>
+      </c>
+      <c r="C769" t="s">
+        <v>2177</v>
+      </c>
+      <c r="D769" t="s">
+        <v>2178</v>
+      </c>
+      <c r="E769" s="2">
+        <v>4</v>
+      </c>
+      <c r="F769" t="s">
+        <v>4</v>
+      </c>
+      <c r="G769" t="s">
+        <v>2179</v>
+      </c>
+      <c r="H769" t="s">
+        <v>1</v>
+      </c>
+      <c r="I769" t="s">
+        <v>2180</v>
+      </c>
+      <c r="J769" t="s">
+        <v>7</v>
+      </c>
+      <c r="K769" s="3"/>
+      <c r="L769" s="3">
+        <v>46008</v>
+      </c>
+      <c r="M769" t="s">
+        <v>7</v>
+      </c>
+      <c r="N769" t="s">
+        <v>8</v>
+      </c>
+      <c r="O769" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="770" spans="1:15">
+      <c r="A770" t="s">
+        <v>2181</v>
+      </c>
+      <c r="B770" t="s">
+        <v>53</v>
+      </c>
+      <c r="C770" t="s">
+        <v>2182</v>
+      </c>
+      <c r="D770" t="s">
+        <v>2183</v>
+      </c>
+      <c r="E770" s="2">
+        <v>4</v>
+      </c>
+      <c r="F770" t="s">
+        <v>4</v>
+      </c>
+      <c r="G770" t="s">
+        <v>2179</v>
+      </c>
+      <c r="H770" t="s">
+        <v>53</v>
+      </c>
+      <c r="I770" t="s">
+        <v>2180</v>
+      </c>
+      <c r="J770" t="s">
+        <v>7</v>
+      </c>
+      <c r="K770" s="3"/>
+      <c r="L770" s="3">
+        <v>46008</v>
+      </c>
+      <c r="M770" t="s">
+        <v>7</v>
+      </c>
+      <c r="N770" t="s">
+        <v>8</v>
+      </c>
+      <c r="O770" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="771" spans="1:15">
+      <c r="A771" t="s">
+        <v>2181</v>
+      </c>
+      <c r="B771" t="s">
+        <v>21</v>
+      </c>
+      <c r="C771" t="s">
+        <v>2184</v>
+      </c>
+      <c r="D771" t="s">
+        <v>2185</v>
+      </c>
+      <c r="E771" s="2">
+        <v>2</v>
+      </c>
+      <c r="F771" t="s">
+        <v>4</v>
+      </c>
+      <c r="G771" t="s">
+        <v>2179</v>
+      </c>
+      <c r="H771" t="s">
+        <v>21</v>
+      </c>
+      <c r="I771" t="s">
+        <v>2180</v>
+      </c>
+      <c r="J771" t="s">
+        <v>7</v>
+      </c>
+      <c r="K771" s="3"/>
+      <c r="L771" s="3">
+        <v>46008</v>
+      </c>
+      <c r="M771" t="s">
+        <v>7</v>
+      </c>
+      <c r="N771" t="s">
+        <v>8</v>
+      </c>
+      <c r="O771" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="772" spans="1:15">
+      <c r="A772" t="s">
+        <v>2186</v>
+      </c>
+      <c r="B772" t="s">
+        <v>1</v>
+      </c>
+      <c r="C772" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D772" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E772" s="2">
+        <v>0</v>
+      </c>
+      <c r="F772" t="s">
+        <v>4</v>
+      </c>
+      <c r="G772" t="s">
+        <v>2187</v>
+      </c>
+      <c r="H772" t="s">
+        <v>1</v>
+      </c>
+      <c r="I772" t="s">
+        <v>2188</v>
+      </c>
+      <c r="J772" t="s">
+        <v>7</v>
+      </c>
+      <c r="K772" s="3"/>
+      <c r="L772" s="3">
+        <v>46009</v>
+      </c>
+      <c r="M772" t="s">
+        <v>7</v>
+      </c>
+      <c r="N772" t="s">
+        <v>8</v>
+      </c>
+      <c r="O772" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="773" spans="1:15">
+      <c r="A773" t="s">
+        <v>2189</v>
+      </c>
+      <c r="B773" t="s">
+        <v>1</v>
+      </c>
+      <c r="C773" t="s">
+        <v>2148</v>
+      </c>
+      <c r="D773" t="s">
+        <v>2149</v>
+      </c>
+      <c r="E773" s="2">
+        <v>25</v>
+      </c>
+      <c r="F773" t="s">
+        <v>4</v>
+      </c>
+      <c r="G773" t="s">
+        <v>2190</v>
+      </c>
+      <c r="H773" t="s">
+        <v>1</v>
+      </c>
+      <c r="I773" t="s">
+        <v>2191</v>
+      </c>
+      <c r="J773" t="s">
+        <v>7</v>
+      </c>
+      <c r="K773" s="3"/>
+      <c r="L773" s="3">
+        <v>46013</v>
+      </c>
+      <c r="M773" t="s">
+        <v>7</v>
+      </c>
+      <c r="N773" t="s">
+        <v>8</v>
+      </c>
+      <c r="O773" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="774" spans="1:15">
+      <c r="A774" t="s">
+        <v>2189</v>
+      </c>
+      <c r="B774" t="s">
+        <v>53</v>
+      </c>
+      <c r="C774" t="s">
+        <v>2116</v>
+      </c>
+      <c r="D774" t="s">
+        <v>2117</v>
+      </c>
+      <c r="E774" s="2">
+        <v>25</v>
+      </c>
+      <c r="F774" t="s">
+        <v>4</v>
+      </c>
+      <c r="G774" t="s">
+        <v>2190</v>
+      </c>
+      <c r="H774" t="s">
+        <v>53</v>
+      </c>
+      <c r="I774" t="s">
+        <v>2191</v>
+      </c>
+      <c r="J774" t="s">
+        <v>7</v>
+      </c>
+      <c r="K774" s="3"/>
+      <c r="L774" s="3">
+        <v>46013</v>
+      </c>
+      <c r="M774" t="s">
+        <v>7</v>
+      </c>
+      <c r="N774" t="s">
+        <v>8</v>
+      </c>
+      <c r="O774" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="775" spans="1:15">
+      <c r="A775" t="s">
+        <v>2192</v>
+      </c>
+      <c r="B775" t="s">
+        <v>53</v>
+      </c>
+      <c r="C775" t="s">
+        <v>618</v>
+      </c>
+      <c r="D775" t="s">
+        <v>619</v>
+      </c>
+      <c r="E775" s="2">
+        <v>138</v>
+      </c>
+      <c r="F775" t="s">
+        <v>4</v>
+      </c>
+      <c r="G775" t="s">
+        <v>1927</v>
+      </c>
+      <c r="H775" t="s">
+        <v>53</v>
+      </c>
+      <c r="I775" t="s">
+        <v>2193</v>
+      </c>
+      <c r="J775" t="s">
+        <v>7</v>
+      </c>
+      <c r="K775" s="3"/>
+      <c r="L775" s="3">
+        <v>46027</v>
+      </c>
+      <c r="M775" t="s">
+        <v>7</v>
+      </c>
+      <c r="N775" t="s">
+        <v>8</v>
+      </c>
+      <c r="O775" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="776" spans="1:15">
+      <c r="A776" t="s">
+        <v>2194</v>
+      </c>
+      <c r="B776" t="s">
+        <v>1</v>
+      </c>
+      <c r="C776" t="s">
+        <v>172</v>
+      </c>
+      <c r="D776" t="s">
+        <v>173</v>
+      </c>
+      <c r="E776" s="2">
+        <v>1</v>
+      </c>
+      <c r="F776" t="s">
+        <v>4</v>
+      </c>
+      <c r="G776" t="s">
+        <v>2195</v>
+      </c>
+      <c r="H776" t="s">
+        <v>1</v>
+      </c>
+      <c r="I776" t="s">
+        <v>2196</v>
+      </c>
+      <c r="J776" t="s">
+        <v>7</v>
+      </c>
+      <c r="K776" s="3"/>
+      <c r="L776" s="3">
+        <v>46027</v>
+      </c>
+      <c r="M776" t="s">
+        <v>7</v>
+      </c>
+      <c r="N776" t="s">
+        <v>8</v>
+      </c>
+      <c r="O776" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="777" spans="1:15">
+      <c r="A777" t="s">
+        <v>2197</v>
+      </c>
+      <c r="B777" t="s">
+        <v>1</v>
+      </c>
+      <c r="C777" t="s">
+        <v>444</v>
+      </c>
+      <c r="D777" t="s">
+        <v>445</v>
+      </c>
+      <c r="E777" s="2">
+        <v>30</v>
+      </c>
+      <c r="F777" t="s">
+        <v>4</v>
+      </c>
+      <c r="G777" t="s">
+        <v>2198</v>
+      </c>
+      <c r="H777" t="s">
+        <v>1</v>
+      </c>
+      <c r="I777" t="s">
+        <v>1936</v>
+      </c>
+      <c r="J777" t="s">
+        <v>7</v>
+      </c>
+      <c r="K777" s="3"/>
+      <c r="L777" s="3">
+        <v>46027</v>
+      </c>
+      <c r="M777" t="s">
+        <v>7</v>
+      </c>
+      <c r="N777" t="s">
+        <v>8</v>
+      </c>
+      <c r="O777" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="778" spans="1:15">
+      <c r="A778" t="s">
+        <v>2199</v>
+      </c>
+      <c r="B778" t="s">
+        <v>1</v>
+      </c>
+      <c r="C778" t="s">
+        <v>1173</v>
+      </c>
+      <c r="D778" t="s">
+        <v>1174</v>
+      </c>
+      <c r="E778" s="2">
+        <v>25</v>
+      </c>
+      <c r="F778" t="s">
+        <v>4</v>
+      </c>
+      <c r="G778" t="s">
+        <v>2187</v>
+      </c>
+      <c r="H778" t="s">
+        <v>1</v>
+      </c>
+      <c r="I778" t="s">
+        <v>2188</v>
+      </c>
+      <c r="J778" t="s">
+        <v>7</v>
+      </c>
+      <c r="K778" s="3"/>
+      <c r="L778" s="3">
+        <v>46027</v>
+      </c>
+      <c r="M778" t="s">
+        <v>7</v>
+      </c>
+      <c r="N778" t="s">
+        <v>8</v>
+      </c>
+      <c r="O778" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="779" spans="1:15">
+      <c r="A779" t="s">
+        <v>2200</v>
+      </c>
+      <c r="B779" t="s">
+        <v>21</v>
+      </c>
+      <c r="C779" t="s">
+        <v>991</v>
+      </c>
+      <c r="D779" t="s">
+        <v>992</v>
+      </c>
+      <c r="E779" s="2">
+        <v>51</v>
+      </c>
+      <c r="F779" t="s">
+        <v>4</v>
+      </c>
+      <c r="G779" t="s">
+        <v>2014</v>
+      </c>
+      <c r="H779" t="s">
+        <v>21</v>
+      </c>
+      <c r="I779" t="s">
+        <v>2112</v>
+      </c>
+      <c r="J779" t="s">
+        <v>7</v>
+      </c>
+      <c r="K779" s="3"/>
+      <c r="L779" s="3">
+        <v>46027</v>
+      </c>
+      <c r="M779" t="s">
+        <v>7</v>
+      </c>
+      <c r="N779" t="s">
+        <v>8</v>
+      </c>
+      <c r="O779" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="780" spans="1:15">
+      <c r="A780" t="s">
+        <v>2201</v>
+      </c>
+      <c r="B780" t="s">
+        <v>25</v>
+      </c>
+      <c r="C780" t="s">
+        <v>892</v>
+      </c>
+      <c r="D780" t="s">
+        <v>893</v>
+      </c>
+      <c r="E780" s="2">
+        <v>51</v>
+      </c>
+      <c r="F780" t="s">
+        <v>4</v>
+      </c>
+      <c r="G780" t="s">
+        <v>2014</v>
+      </c>
+      <c r="H780" t="s">
+        <v>25</v>
+      </c>
+      <c r="I780" t="s">
+        <v>2114</v>
+      </c>
+      <c r="J780" t="s">
+        <v>7</v>
+      </c>
+      <c r="K780" s="3"/>
+      <c r="L780" s="3">
+        <v>46027</v>
+      </c>
+      <c r="M780" t="s">
+        <v>7</v>
+      </c>
+      <c r="N780" t="s">
+        <v>8</v>
+      </c>
+      <c r="O780" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="781" spans="1:15">
+      <c r="A781" t="s">
+        <v>2201</v>
+      </c>
+      <c r="B781" t="s">
+        <v>73</v>
+      </c>
+      <c r="C781" t="s">
+        <v>1313</v>
+      </c>
+      <c r="D781" t="s">
+        <v>1314</v>
+      </c>
+      <c r="E781" s="2">
+        <v>75</v>
+      </c>
+      <c r="F781" t="s">
+        <v>4</v>
+      </c>
+      <c r="G781" t="s">
+        <v>2014</v>
+      </c>
+      <c r="H781" t="s">
+        <v>73</v>
+      </c>
+      <c r="I781" t="s">
+        <v>2114</v>
+      </c>
+      <c r="J781" t="s">
+        <v>7</v>
+      </c>
+      <c r="K781" s="3"/>
+      <c r="L781" s="3">
+        <v>46027</v>
+      </c>
+      <c r="M781" t="s">
+        <v>7</v>
+      </c>
+      <c r="N781" t="s">
+        <v>8</v>
+      </c>
+      <c r="O781" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="782" spans="1:15">
+      <c r="A782" t="s">
+        <v>2201</v>
+      </c>
+      <c r="B782" t="s">
+        <v>79</v>
+      </c>
+      <c r="C782" t="s">
+        <v>952</v>
+      </c>
+      <c r="D782" t="s">
+        <v>953</v>
+      </c>
+      <c r="E782" s="2">
+        <v>40</v>
+      </c>
+      <c r="F782" t="s">
+        <v>4</v>
+      </c>
+      <c r="G782" t="s">
+        <v>2014</v>
+      </c>
+      <c r="H782" t="s">
+        <v>79</v>
+      </c>
+      <c r="I782" t="s">
+        <v>2114</v>
+      </c>
+      <c r="J782" t="s">
+        <v>7</v>
+      </c>
+      <c r="K782" s="3"/>
+      <c r="L782" s="3">
+        <v>46027</v>
+      </c>
+      <c r="M782" t="s">
+        <v>7</v>
+      </c>
+      <c r="N782" t="s">
+        <v>8</v>
+      </c>
+      <c r="O782" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="783" spans="1:15">
+      <c r="A783" t="s">
+        <v>2201</v>
+      </c>
+      <c r="B783" t="s">
+        <v>357</v>
+      </c>
+      <c r="C783" t="s">
+        <v>1573</v>
+      </c>
+      <c r="D783" t="s">
+        <v>1574</v>
+      </c>
+      <c r="E783" s="2">
+        <v>15</v>
+      </c>
+      <c r="F783" t="s">
+        <v>4</v>
+      </c>
+      <c r="G783" t="s">
+        <v>2014</v>
+      </c>
+      <c r="H783" t="s">
+        <v>357</v>
+      </c>
+      <c r="I783" t="s">
+        <v>2114</v>
+      </c>
+      <c r="J783" t="s">
+        <v>7</v>
+      </c>
+      <c r="K783" s="3"/>
+      <c r="L783" s="3">
+        <v>46027</v>
+      </c>
+      <c r="M783" t="s">
+        <v>7</v>
+      </c>
+      <c r="N783" t="s">
+        <v>8</v>
+      </c>
+      <c r="O783" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="784" spans="1:15">
+      <c r="A784" t="s">
+        <v>2202</v>
+      </c>
+      <c r="B784" t="s">
+        <v>1</v>
+      </c>
+      <c r="C784" t="s">
+        <v>461</v>
+      </c>
+      <c r="D784" t="s">
+        <v>462</v>
+      </c>
+      <c r="E784" s="2">
+        <v>16</v>
+      </c>
+      <c r="F784" t="s">
+        <v>4</v>
+      </c>
+      <c r="G784" t="s">
+        <v>2029</v>
+      </c>
+      <c r="H784" t="s">
+        <v>1</v>
+      </c>
+      <c r="I784" t="s">
+        <v>2203</v>
+      </c>
+      <c r="J784" t="s">
+        <v>7</v>
+      </c>
+      <c r="K784" s="3"/>
+      <c r="L784" s="3">
+        <v>46028</v>
+      </c>
+      <c r="M784" t="s">
+        <v>7</v>
+      </c>
+      <c r="N784" t="s">
+        <v>8</v>
+      </c>
+      <c r="O784" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="785" spans="1:15">
+      <c r="A785" t="s">
+        <v>2204</v>
+      </c>
+      <c r="B785" t="s">
+        <v>53</v>
+      </c>
+      <c r="C785" t="s">
+        <v>278</v>
+      </c>
+      <c r="D785" t="s">
+        <v>279</v>
+      </c>
+      <c r="E785" s="2">
+        <v>20</v>
+      </c>
+      <c r="F785" t="s">
+        <v>4</v>
+      </c>
+      <c r="G785" t="s">
+        <v>1578</v>
+      </c>
+      <c r="H785" t="s">
+        <v>53</v>
+      </c>
+      <c r="I785" t="s">
+        <v>2205</v>
+      </c>
+      <c r="J785" t="s">
+        <v>7</v>
+      </c>
+      <c r="K785" s="3"/>
+      <c r="L785" s="3">
+        <v>46028</v>
+      </c>
+      <c r="M785" t="s">
+        <v>7</v>
+      </c>
+      <c r="N785" t="s">
+        <v>8</v>
+      </c>
+      <c r="O785" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="786" spans="1:15">
+      <c r="A786" t="s">
+        <v>2206</v>
+      </c>
+      <c r="B786" t="s">
+        <v>1</v>
+      </c>
+      <c r="C786" t="s">
+        <v>600</v>
+      </c>
+      <c r="D786" t="s">
+        <v>601</v>
+      </c>
+      <c r="E786" s="2">
+        <v>10</v>
+      </c>
+      <c r="F786" t="s">
+        <v>4</v>
+      </c>
+      <c r="G786" t="s">
+        <v>1969</v>
+      </c>
+      <c r="H786" t="s">
+        <v>1</v>
+      </c>
+      <c r="I786" t="s">
+        <v>2207</v>
+      </c>
+      <c r="J786" t="s">
+        <v>7</v>
+      </c>
+      <c r="K786" s="3"/>
+      <c r="L786" s="3">
+        <v>46028</v>
+      </c>
+      <c r="M786" t="s">
+        <v>7</v>
+      </c>
+      <c r="N786" t="s">
+        <v>8</v>
+      </c>
+      <c r="O786" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="787" spans="1:15">
+      <c r="A787" t="s">
+        <v>2208</v>
+      </c>
+      <c r="B787" t="s">
+        <v>1</v>
+      </c>
+      <c r="C787" t="s">
+        <v>451</v>
+      </c>
+      <c r="D787" t="s">
+        <v>452</v>
+      </c>
+      <c r="E787" s="2">
+        <v>160</v>
+      </c>
+      <c r="F787" t="s">
+        <v>4</v>
+      </c>
+      <c r="G787" t="s">
+        <v>1768</v>
+      </c>
+      <c r="H787" t="s">
+        <v>1</v>
+      </c>
+      <c r="I787" t="s">
+        <v>2209</v>
+      </c>
+      <c r="J787" t="s">
+        <v>7</v>
+      </c>
+      <c r="K787" s="3"/>
+      <c r="L787" s="3">
+        <v>46028</v>
+      </c>
+      <c r="M787" t="s">
+        <v>7</v>
+      </c>
+      <c r="N787" t="s">
+        <v>8</v>
+      </c>
+      <c r="O787" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="788" spans="1:15">
+      <c r="A788" t="s">
+        <v>2210</v>
+      </c>
+      <c r="B788" t="s">
+        <v>1</v>
+      </c>
+      <c r="C788" t="s">
+        <v>312</v>
+      </c>
+      <c r="D788" t="s">
+        <v>313</v>
+      </c>
+      <c r="E788" s="2">
+        <v>25</v>
+      </c>
+      <c r="F788" t="s">
+        <v>4</v>
+      </c>
+      <c r="G788" t="s">
+        <v>1761</v>
+      </c>
+      <c r="H788" t="s">
+        <v>1</v>
+      </c>
+      <c r="I788" t="s">
+        <v>124</v>
+      </c>
+      <c r="J788" t="s">
+        <v>7</v>
+      </c>
+      <c r="K788" s="3"/>
+      <c r="L788" s="3">
+        <v>46028</v>
+      </c>
+      <c r="M788" t="s">
+        <v>7</v>
+      </c>
+      <c r="N788" t="s">
+        <v>8</v>
+      </c>
+      <c r="O788" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="789" spans="1:15">
+      <c r="A789" t="s">
+        <v>2211</v>
+      </c>
+      <c r="B789" t="s">
+        <v>1</v>
+      </c>
+      <c r="C789" t="s">
+        <v>1585</v>
+      </c>
+      <c r="D789" t="s">
+        <v>1586</v>
+      </c>
+      <c r="E789" s="2">
+        <v>31</v>
+      </c>
+      <c r="F789" t="s">
+        <v>4</v>
+      </c>
+      <c r="G789" t="s">
+        <v>2014</v>
+      </c>
+      <c r="H789" t="s">
+        <v>1</v>
+      </c>
+      <c r="I789" t="s">
+        <v>2039</v>
+      </c>
+      <c r="J789" t="s">
+        <v>7</v>
+      </c>
+      <c r="K789" s="3"/>
+      <c r="L789" s="3">
+        <v>46028</v>
+      </c>
+      <c r="M789" t="s">
+        <v>2169</v>
+      </c>
+      <c r="N789" t="s">
+        <v>8</v>
+      </c>
+      <c r="O789" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="790" spans="1:15">
+      <c r="A790" t="s">
+        <v>2211</v>
+      </c>
+      <c r="B790" t="s">
+        <v>76</v>
+      </c>
+      <c r="C790" t="s">
+        <v>937</v>
+      </c>
+      <c r="D790" t="s">
+        <v>938</v>
+      </c>
+      <c r="E790" s="2">
+        <v>40</v>
+      </c>
+      <c r="F790" t="s">
+        <v>4</v>
+      </c>
+      <c r="G790" t="s">
+        <v>2014</v>
+      </c>
+      <c r="H790" t="s">
+        <v>76</v>
+      </c>
+      <c r="I790" t="s">
+        <v>2039</v>
+      </c>
+      <c r="J790" t="s">
+        <v>7</v>
+      </c>
+      <c r="K790" s="3"/>
+      <c r="L790" s="3">
+        <v>46028</v>
+      </c>
+      <c r="M790" t="s">
+        <v>2169</v>
+      </c>
+      <c r="N790" t="s">
+        <v>8</v>
+      </c>
+      <c r="O790" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="791" spans="1:15">
+      <c r="A791" t="s">
+        <v>2211</v>
+      </c>
+      <c r="B791" t="s">
+        <v>344</v>
+      </c>
+      <c r="C791" t="s">
+        <v>1635</v>
+      </c>
+      <c r="D791" t="s">
+        <v>1636</v>
+      </c>
+      <c r="E791" s="2">
+        <v>25</v>
+      </c>
+      <c r="F791" t="s">
+        <v>4</v>
+      </c>
+      <c r="G791" t="s">
+        <v>2014</v>
+      </c>
+      <c r="H791" t="s">
+        <v>344</v>
+      </c>
+      <c r="I791" t="s">
+        <v>2039</v>
+      </c>
+      <c r="J791" t="s">
+        <v>7</v>
+      </c>
+      <c r="K791" s="3"/>
+      <c r="L791" s="3">
+        <v>46028</v>
+      </c>
+      <c r="M791" t="s">
+        <v>2169</v>
+      </c>
+      <c r="N791" t="s">
+        <v>8</v>
+      </c>
+      <c r="O791" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="792" spans="1:15">
+      <c r="A792" t="s">
+        <v>2212</v>
+      </c>
+      <c r="B792" t="s">
+        <v>1</v>
+      </c>
+      <c r="C792" t="s">
+        <v>1930</v>
+      </c>
+      <c r="D792" t="s">
+        <v>1931</v>
+      </c>
+      <c r="E792" s="2">
+        <v>24</v>
+      </c>
+      <c r="F792" t="s">
+        <v>4</v>
+      </c>
+      <c r="G792" t="s">
+        <v>1932</v>
+      </c>
+      <c r="H792" t="s">
+        <v>1</v>
+      </c>
+      <c r="I792" t="s">
+        <v>2213</v>
+      </c>
+      <c r="J792" t="s">
+        <v>7</v>
+      </c>
+      <c r="K792" s="3"/>
+      <c r="L792" s="3">
+        <v>46028</v>
+      </c>
+      <c r="M792" t="s">
+        <v>2169</v>
+      </c>
+      <c r="N792" t="s">
+        <v>8</v>
+      </c>
+      <c r="O792" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="793" spans="1:15">
+      <c r="A793" t="s">
+        <v>2214</v>
+      </c>
+      <c r="B793" t="s">
+        <v>1</v>
+      </c>
+      <c r="C793" t="s">
+        <v>203</v>
+      </c>
+      <c r="D793" t="s">
+        <v>204</v>
+      </c>
+      <c r="E793" s="2">
+        <v>40</v>
+      </c>
+      <c r="F793" t="s">
+        <v>4</v>
+      </c>
+      <c r="G793" t="s">
+        <v>1763</v>
+      </c>
+      <c r="H793" t="s">
+        <v>1</v>
+      </c>
+      <c r="I793" t="s">
+        <v>2215</v>
+      </c>
+      <c r="J793" t="s">
+        <v>7</v>
+      </c>
+      <c r="K793" s="3"/>
+      <c r="L793" s="3">
+        <v>46028</v>
+      </c>
+      <c r="M793" t="s">
+        <v>2169</v>
+      </c>
+      <c r="N793" t="s">
+        <v>8</v>
+      </c>
+      <c r="O793" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="794" spans="1:15">
+      <c r="A794" t="s">
+        <v>2216</v>
+      </c>
+      <c r="B794" t="s">
+        <v>1</v>
+      </c>
+      <c r="C794" t="s">
+        <v>614</v>
+      </c>
+      <c r="D794" t="s">
+        <v>615</v>
+      </c>
+      <c r="E794" s="2">
+        <v>17</v>
+      </c>
+      <c r="F794" t="s">
+        <v>4</v>
+      </c>
+      <c r="G794" t="s">
+        <v>1784</v>
+      </c>
+      <c r="H794" t="s">
+        <v>1</v>
+      </c>
+      <c r="I794" t="s">
+        <v>2217</v>
+      </c>
+      <c r="J794" t="s">
+        <v>7</v>
+      </c>
+      <c r="K794" s="3"/>
+      <c r="L794" s="3">
+        <v>46028</v>
+      </c>
+      <c r="M794" t="s">
+        <v>2169</v>
+      </c>
+      <c r="N794" t="s">
+        <v>8</v>
+      </c>
+      <c r="O794" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="795" spans="1:15">
+      <c r="A795" t="s">
+        <v>2216</v>
+      </c>
+      <c r="B795" t="s">
+        <v>21</v>
+      </c>
+      <c r="C795" t="s">
+        <v>1786</v>
+      </c>
+      <c r="D795" t="s">
+        <v>1787</v>
+      </c>
+      <c r="E795" s="2">
+        <v>7</v>
+      </c>
+      <c r="F795" t="s">
+        <v>4</v>
+      </c>
+      <c r="G795" t="s">
+        <v>1784</v>
+      </c>
+      <c r="H795" t="s">
+        <v>21</v>
+      </c>
+      <c r="I795" t="s">
+        <v>2217</v>
+      </c>
+      <c r="J795" t="s">
+        <v>7</v>
+      </c>
+      <c r="K795" s="3"/>
+      <c r="L795" s="3">
+        <v>46028</v>
+      </c>
+      <c r="M795" t="s">
+        <v>2169</v>
+      </c>
+      <c r="N795" t="s">
+        <v>8</v>
+      </c>
+      <c r="O795" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deploy: i18n, period mode, duplicate handling, layout chunk fix, docs, metrics note
- Full i18n for period mode, Change History, filter warning, month names (en/de/it)
- Period mode (12MB/YTD) on Dashboard, PPAPs, Deviations, Cost Poor Quality, Audit Management, Warranties Costs
- Upload merge + dedupe by id; duplicate badge and Change History filter
- Layout chunk fix (ThemeProvider/toaster); fallback Retry on ChunkLoadError
- Plant filter from Webasto ET Plants only; dashboard metrics note when sites selected
- Documentation: CHANGELOG, MEMORY_BANK, PROJECT_STATE, AUDIT, EVALUATION, DOCUMENTATION_INDEX
- API/complaints, Prisma, repo abstraction, new docs

Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/attachments/Inbound 411_PS4.XLSX
+++ b/attachments/Inbound 411_PS4.XLSX
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9543" uniqueCount="2233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10071" uniqueCount="2319">
   <si>
     <t>180104337</t>
   </si>
@@ -6520,9 +6520,6 @@
     <t>180136240</t>
   </si>
   <si>
-    <t>Not Started</t>
-  </si>
-  <si>
     <t>180136393</t>
   </si>
   <si>
@@ -6665,6 +6662,267 @@
   </si>
   <si>
     <t>ACPF</t>
+  </si>
+  <si>
+    <t>180137208</t>
+  </si>
+  <si>
+    <t>4500032235</t>
+  </si>
+  <si>
+    <t>180137209</t>
+  </si>
+  <si>
+    <t>109225</t>
+  </si>
+  <si>
+    <t>180137319</t>
+  </si>
+  <si>
+    <t>61055</t>
+  </si>
+  <si>
+    <t>180137320</t>
+  </si>
+  <si>
+    <t>61022</t>
+  </si>
+  <si>
+    <t>180137328</t>
+  </si>
+  <si>
+    <t>109223</t>
+  </si>
+  <si>
+    <t>180137329</t>
+  </si>
+  <si>
+    <t>109222</t>
+  </si>
+  <si>
+    <t>180137330</t>
+  </si>
+  <si>
+    <t>109226</t>
+  </si>
+  <si>
+    <t>180137331</t>
+  </si>
+  <si>
+    <t>109220</t>
+  </si>
+  <si>
+    <t>180137332</t>
+  </si>
+  <si>
+    <t>109221</t>
+  </si>
+  <si>
+    <t>180137333</t>
+  </si>
+  <si>
+    <t>109219</t>
+  </si>
+  <si>
+    <t>08484-C</t>
+  </si>
+  <si>
+    <t>CBL ASSY 85inL POWERSTAGE POWER SUPPLY</t>
+  </si>
+  <si>
+    <t>23175-04</t>
+  </si>
+  <si>
+    <t>CBL ASSY EMERGANCY PWR OFF MONITOR 900</t>
+  </si>
+  <si>
+    <t>180137334</t>
+  </si>
+  <si>
+    <t>109224</t>
+  </si>
+  <si>
+    <t>180137337</t>
+  </si>
+  <si>
+    <t>109219-2</t>
+  </si>
+  <si>
+    <t>180137369</t>
+  </si>
+  <si>
+    <t>109227</t>
+  </si>
+  <si>
+    <t>180137375</t>
+  </si>
+  <si>
+    <t>180137386</t>
+  </si>
+  <si>
+    <t>61053</t>
+  </si>
+  <si>
+    <t>23853-04</t>
+  </si>
+  <si>
+    <t>CBL ASSY H2 CONTROL XFMR-PS1 LINE 900 EX</t>
+  </si>
+  <si>
+    <t>180137387</t>
+  </si>
+  <si>
+    <t>109232</t>
+  </si>
+  <si>
+    <t>180137495</t>
+  </si>
+  <si>
+    <t>5913358A</t>
+  </si>
+  <si>
+    <t>PCBA PWR AC INVERTER 900</t>
+  </si>
+  <si>
+    <t>4500025391</t>
+  </si>
+  <si>
+    <t>36841</t>
+  </si>
+  <si>
+    <t>180137757</t>
+  </si>
+  <si>
+    <t>23484-02</t>
+  </si>
+  <si>
+    <t>CRATE WOOD POWER STAGE 900</t>
+  </si>
+  <si>
+    <t>4500032411</t>
+  </si>
+  <si>
+    <t>1/12/2026</t>
+  </si>
+  <si>
+    <t>180137759</t>
+  </si>
+  <si>
+    <t>192435</t>
+  </si>
+  <si>
+    <t>07052-C</t>
+  </si>
+  <si>
+    <t>SPACER RECT BLOCK 0.5inx2inx2.5in 900</t>
+  </si>
+  <si>
+    <t>180137760</t>
+  </si>
+  <si>
+    <t>180137983</t>
+  </si>
+  <si>
+    <t>109249</t>
+  </si>
+  <si>
+    <t>180138390</t>
+  </si>
+  <si>
+    <t>4500032193</t>
+  </si>
+  <si>
+    <t>109262</t>
+  </si>
+  <si>
+    <t>180138391</t>
+  </si>
+  <si>
+    <t>109254</t>
+  </si>
+  <si>
+    <t>180138392</t>
+  </si>
+  <si>
+    <t>109260</t>
+  </si>
+  <si>
+    <t>180138393</t>
+  </si>
+  <si>
+    <t>4500029852</t>
+  </si>
+  <si>
+    <t>2106643927</t>
+  </si>
+  <si>
+    <t>180138394</t>
+  </si>
+  <si>
+    <t>4500030372</t>
+  </si>
+  <si>
+    <t>61119</t>
+  </si>
+  <si>
+    <t>180138395</t>
+  </si>
+  <si>
+    <t>61131</t>
+  </si>
+  <si>
+    <t>180138787</t>
+  </si>
+  <si>
+    <t>23298-03</t>
+  </si>
+  <si>
+    <t>CBL ASY DC CONT CNTL II 900</t>
+  </si>
+  <si>
+    <t>61142</t>
+  </si>
+  <si>
+    <t>180138788</t>
+  </si>
+  <si>
+    <t>4500033522</t>
+  </si>
+  <si>
+    <t>1241964-01</t>
+  </si>
+  <si>
+    <t>180138797</t>
+  </si>
+  <si>
+    <t>4500032240</t>
+  </si>
+  <si>
+    <t>677990</t>
+  </si>
+  <si>
+    <t>180138991</t>
+  </si>
+  <si>
+    <t>4500033664</t>
+  </si>
+  <si>
+    <t>180139182</t>
+  </si>
+  <si>
+    <t>4500033792</t>
+  </si>
+  <si>
+    <t>1/22/2026</t>
+  </si>
+  <si>
+    <t>180139185</t>
+  </si>
+  <si>
+    <t>180139452</t>
+  </si>
+  <si>
+    <t>34056</t>
   </si>
   <si>
     <t>Document</t>
@@ -6814,7 +7072,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O795"/>
+  <dimension ref="A1:O839"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6841,49 +7099,49 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
-        <v>2218</v>
+        <v>2304</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2219</v>
+        <v>2305</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2220</v>
+        <v>2306</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2221</v>
+        <v>2307</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2222</v>
+        <v>2308</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>2223</v>
+        <v>2309</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>2224</v>
+        <v>2310</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>2225</v>
+        <v>2311</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>2226</v>
+        <v>2312</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>2227</v>
+        <v>2313</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>2228</v>
+        <v>2314</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>2229</v>
+        <v>2315</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>2230</v>
+        <v>2316</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>2231</v>
+        <v>2317</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>2232</v>
+        <v>2318</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -41185,7 +41443,7 @@
         <v>46006</v>
       </c>
       <c r="M763" t="s">
-        <v>2169</v>
+        <v>7</v>
       </c>
       <c r="N763" t="s">
         <v>8</v>
@@ -41196,7 +41454,7 @@
     </row>
     <row r="764" spans="1:15">
       <c r="A764" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="B764" t="s">
         <v>1</v>
@@ -41214,13 +41472,13 @@
         <v>4</v>
       </c>
       <c r="G764" t="s">
+        <v>2170</v>
+      </c>
+      <c r="H764" t="s">
+        <v>1</v>
+      </c>
+      <c r="I764" t="s">
         <v>2171</v>
-      </c>
-      <c r="H764" t="s">
-        <v>1</v>
-      </c>
-      <c r="I764" t="s">
-        <v>2172</v>
       </c>
       <c r="J764" t="s">
         <v>7</v>
@@ -41241,7 +41499,7 @@
     </row>
     <row r="765" spans="1:15">
       <c r="A765" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="B765" t="s">
         <v>53</v>
@@ -41259,13 +41517,13 @@
         <v>4</v>
       </c>
       <c r="G765" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="H765" t="s">
         <v>53</v>
       </c>
       <c r="I765" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="J765" t="s">
         <v>7</v>
@@ -41286,7 +41544,7 @@
     </row>
     <row r="766" spans="1:15">
       <c r="A766" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="B766" t="s">
         <v>21</v>
@@ -41304,13 +41562,13 @@
         <v>4</v>
       </c>
       <c r="G766" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="H766" t="s">
         <v>21</v>
       </c>
       <c r="I766" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="J766" t="s">
         <v>7</v>
@@ -41331,7 +41589,7 @@
     </row>
     <row r="767" spans="1:15">
       <c r="A767" t="s">
-        <v>2170</v>
+        <v>2169</v>
       </c>
       <c r="B767" t="s">
         <v>25</v>
@@ -41349,13 +41607,13 @@
         <v>4</v>
       </c>
       <c r="G767" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="H767" t="s">
         <v>25</v>
       </c>
       <c r="I767" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="J767" t="s">
         <v>7</v>
@@ -41376,7 +41634,7 @@
     </row>
     <row r="768" spans="1:15">
       <c r="A768" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
       <c r="B768" t="s">
         <v>1</v>
@@ -41394,13 +41652,13 @@
         <v>4</v>
       </c>
       <c r="G768" t="s">
+        <v>2173</v>
+      </c>
+      <c r="H768" t="s">
+        <v>1</v>
+      </c>
+      <c r="I768" t="s">
         <v>2174</v>
-      </c>
-      <c r="H768" t="s">
-        <v>1</v>
-      </c>
-      <c r="I768" t="s">
-        <v>2175</v>
       </c>
       <c r="J768" t="s">
         <v>7</v>
@@ -41421,31 +41679,31 @@
     </row>
     <row r="769" spans="1:15">
       <c r="A769" t="s">
+        <v>2175</v>
+      </c>
+      <c r="B769" t="s">
+        <v>1</v>
+      </c>
+      <c r="C769" t="s">
         <v>2176</v>
       </c>
-      <c r="B769" t="s">
-        <v>1</v>
-      </c>
-      <c r="C769" t="s">
+      <c r="D769" t="s">
         <v>2177</v>
       </c>
-      <c r="D769" t="s">
+      <c r="E769" s="2">
+        <v>4</v>
+      </c>
+      <c r="F769" t="s">
+        <v>4</v>
+      </c>
+      <c r="G769" t="s">
         <v>2178</v>
       </c>
-      <c r="E769" s="2">
-        <v>4</v>
-      </c>
-      <c r="F769" t="s">
-        <v>4</v>
-      </c>
-      <c r="G769" t="s">
+      <c r="H769" t="s">
+        <v>1</v>
+      </c>
+      <c r="I769" t="s">
         <v>2179</v>
-      </c>
-      <c r="H769" t="s">
-        <v>1</v>
-      </c>
-      <c r="I769" t="s">
-        <v>2180</v>
       </c>
       <c r="J769" t="s">
         <v>7</v>
@@ -41466,17 +41724,17 @@
     </row>
     <row r="770" spans="1:15">
       <c r="A770" t="s">
-        <v>2181</v>
+        <v>2180</v>
       </c>
       <c r="B770" t="s">
         <v>53</v>
       </c>
       <c r="C770" t="s">
+        <v>2181</v>
+      </c>
+      <c r="D770" t="s">
         <v>2182</v>
       </c>
-      <c r="D770" t="s">
-        <v>2183</v>
-      </c>
       <c r="E770" s="2">
         <v>4</v>
       </c>
@@ -41484,13 +41742,13 @@
         <v>4</v>
       </c>
       <c r="G770" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="H770" t="s">
         <v>53</v>
       </c>
       <c r="I770" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
       <c r="J770" t="s">
         <v>7</v>
@@ -41511,16 +41769,16 @@
     </row>
     <row r="771" spans="1:15">
       <c r="A771" t="s">
-        <v>2181</v>
+        <v>2180</v>
       </c>
       <c r="B771" t="s">
         <v>21</v>
       </c>
       <c r="C771" t="s">
+        <v>2183</v>
+      </c>
+      <c r="D771" t="s">
         <v>2184</v>
-      </c>
-      <c r="D771" t="s">
-        <v>2185</v>
       </c>
       <c r="E771" s="2">
         <v>2</v>
@@ -41529,13 +41787,13 @@
         <v>4</v>
       </c>
       <c r="G771" t="s">
-        <v>2179</v>
+        <v>2178</v>
       </c>
       <c r="H771" t="s">
         <v>21</v>
       </c>
       <c r="I771" t="s">
-        <v>2180</v>
+        <v>2179</v>
       </c>
       <c r="J771" t="s">
         <v>7</v>
@@ -41556,7 +41814,7 @@
     </row>
     <row r="772" spans="1:15">
       <c r="A772" t="s">
-        <v>2186</v>
+        <v>2185</v>
       </c>
       <c r="B772" t="s">
         <v>1</v>
@@ -41574,13 +41832,13 @@
         <v>4</v>
       </c>
       <c r="G772" t="s">
+        <v>2186</v>
+      </c>
+      <c r="H772" t="s">
+        <v>1</v>
+      </c>
+      <c r="I772" t="s">
         <v>2187</v>
-      </c>
-      <c r="H772" t="s">
-        <v>1</v>
-      </c>
-      <c r="I772" t="s">
-        <v>2188</v>
       </c>
       <c r="J772" t="s">
         <v>7</v>
@@ -41601,7 +41859,7 @@
     </row>
     <row r="773" spans="1:15">
       <c r="A773" t="s">
-        <v>2189</v>
+        <v>2188</v>
       </c>
       <c r="B773" t="s">
         <v>1</v>
@@ -41619,13 +41877,13 @@
         <v>4</v>
       </c>
       <c r="G773" t="s">
+        <v>2189</v>
+      </c>
+      <c r="H773" t="s">
+        <v>1</v>
+      </c>
+      <c r="I773" t="s">
         <v>2190</v>
-      </c>
-      <c r="H773" t="s">
-        <v>1</v>
-      </c>
-      <c r="I773" t="s">
-        <v>2191</v>
       </c>
       <c r="J773" t="s">
         <v>7</v>
@@ -41646,7 +41904,7 @@
     </row>
     <row r="774" spans="1:15">
       <c r="A774" t="s">
-        <v>2189</v>
+        <v>2188</v>
       </c>
       <c r="B774" t="s">
         <v>53</v>
@@ -41664,13 +41922,13 @@
         <v>4</v>
       </c>
       <c r="G774" t="s">
-        <v>2190</v>
+        <v>2189</v>
       </c>
       <c r="H774" t="s">
         <v>53</v>
       </c>
       <c r="I774" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="J774" t="s">
         <v>7</v>
@@ -41691,7 +41949,7 @@
     </row>
     <row r="775" spans="1:15">
       <c r="A775" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="B775" t="s">
         <v>53</v>
@@ -41715,7 +41973,7 @@
         <v>53</v>
       </c>
       <c r="I775" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="J775" t="s">
         <v>7</v>
@@ -41736,7 +41994,7 @@
     </row>
     <row r="776" spans="1:15">
       <c r="A776" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="B776" t="s">
         <v>1</v>
@@ -41754,13 +42012,13 @@
         <v>4</v>
       </c>
       <c r="G776" t="s">
+        <v>2194</v>
+      </c>
+      <c r="H776" t="s">
+        <v>1</v>
+      </c>
+      <c r="I776" t="s">
         <v>2195</v>
-      </c>
-      <c r="H776" t="s">
-        <v>1</v>
-      </c>
-      <c r="I776" t="s">
-        <v>2196</v>
       </c>
       <c r="J776" t="s">
         <v>7</v>
@@ -41781,7 +42039,7 @@
     </row>
     <row r="777" spans="1:15">
       <c r="A777" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="B777" t="s">
         <v>1</v>
@@ -41799,7 +42057,7 @@
         <v>4</v>
       </c>
       <c r="G777" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="H777" t="s">
         <v>1</v>
@@ -41826,7 +42084,7 @@
     </row>
     <row r="778" spans="1:15">
       <c r="A778" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="B778" t="s">
         <v>1</v>
@@ -41844,13 +42102,13 @@
         <v>4</v>
       </c>
       <c r="G778" t="s">
+        <v>2186</v>
+      </c>
+      <c r="H778" t="s">
+        <v>1</v>
+      </c>
+      <c r="I778" t="s">
         <v>2187</v>
-      </c>
-      <c r="H778" t="s">
-        <v>1</v>
-      </c>
-      <c r="I778" t="s">
-        <v>2188</v>
       </c>
       <c r="J778" t="s">
         <v>7</v>
@@ -41871,7 +42129,7 @@
     </row>
     <row r="779" spans="1:15">
       <c r="A779" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="B779" t="s">
         <v>21</v>
@@ -41916,7 +42174,7 @@
     </row>
     <row r="780" spans="1:15">
       <c r="A780" t="s">
-        <v>2201</v>
+        <v>2200</v>
       </c>
       <c r="B780" t="s">
         <v>25</v>
@@ -41961,7 +42219,7 @@
     </row>
     <row r="781" spans="1:15">
       <c r="A781" t="s">
-        <v>2201</v>
+        <v>2200</v>
       </c>
       <c r="B781" t="s">
         <v>73</v>
@@ -42006,7 +42264,7 @@
     </row>
     <row r="782" spans="1:15">
       <c r="A782" t="s">
-        <v>2201</v>
+        <v>2200</v>
       </c>
       <c r="B782" t="s">
         <v>79</v>
@@ -42051,7 +42309,7 @@
     </row>
     <row r="783" spans="1:15">
       <c r="A783" t="s">
-        <v>2201</v>
+        <v>2200</v>
       </c>
       <c r="B783" t="s">
         <v>357</v>
@@ -42096,7 +42354,7 @@
     </row>
     <row r="784" spans="1:15">
       <c r="A784" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="B784" t="s">
         <v>1</v>
@@ -42120,7 +42378,7 @@
         <v>1</v>
       </c>
       <c r="I784" t="s">
-        <v>2203</v>
+        <v>2202</v>
       </c>
       <c r="J784" t="s">
         <v>7</v>
@@ -42141,7 +42399,7 @@
     </row>
     <row r="785" spans="1:15">
       <c r="A785" t="s">
-        <v>2204</v>
+        <v>2203</v>
       </c>
       <c r="B785" t="s">
         <v>53</v>
@@ -42165,7 +42423,7 @@
         <v>53</v>
       </c>
       <c r="I785" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
       <c r="J785" t="s">
         <v>7</v>
@@ -42186,7 +42444,7 @@
     </row>
     <row r="786" spans="1:15">
       <c r="A786" t="s">
-        <v>2206</v>
+        <v>2205</v>
       </c>
       <c r="B786" t="s">
         <v>1</v>
@@ -42210,7 +42468,7 @@
         <v>1</v>
       </c>
       <c r="I786" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
       <c r="J786" t="s">
         <v>7</v>
@@ -42231,7 +42489,7 @@
     </row>
     <row r="787" spans="1:15">
       <c r="A787" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="B787" t="s">
         <v>1</v>
@@ -42255,7 +42513,7 @@
         <v>1</v>
       </c>
       <c r="I787" t="s">
-        <v>2209</v>
+        <v>2208</v>
       </c>
       <c r="J787" t="s">
         <v>7</v>
@@ -42276,7 +42534,7 @@
     </row>
     <row r="788" spans="1:15">
       <c r="A788" t="s">
-        <v>2210</v>
+        <v>2209</v>
       </c>
       <c r="B788" t="s">
         <v>1</v>
@@ -42321,7 +42579,7 @@
     </row>
     <row r="789" spans="1:15">
       <c r="A789" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
       <c r="B789" t="s">
         <v>1</v>
@@ -42355,7 +42613,7 @@
         <v>46028</v>
       </c>
       <c r="M789" t="s">
-        <v>2169</v>
+        <v>7</v>
       </c>
       <c r="N789" t="s">
         <v>8</v>
@@ -42366,7 +42624,7 @@
     </row>
     <row r="790" spans="1:15">
       <c r="A790" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
       <c r="B790" t="s">
         <v>76</v>
@@ -42400,7 +42658,7 @@
         <v>46028</v>
       </c>
       <c r="M790" t="s">
-        <v>2169</v>
+        <v>7</v>
       </c>
       <c r="N790" t="s">
         <v>8</v>
@@ -42411,7 +42669,7 @@
     </row>
     <row r="791" spans="1:15">
       <c r="A791" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
       <c r="B791" t="s">
         <v>344</v>
@@ -42445,7 +42703,7 @@
         <v>46028</v>
       </c>
       <c r="M791" t="s">
-        <v>2169</v>
+        <v>7</v>
       </c>
       <c r="N791" t="s">
         <v>8</v>
@@ -42456,7 +42714,7 @@
     </row>
     <row r="792" spans="1:15">
       <c r="A792" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
       <c r="B792" t="s">
         <v>1</v>
@@ -42480,7 +42738,7 @@
         <v>1</v>
       </c>
       <c r="I792" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
       <c r="J792" t="s">
         <v>7</v>
@@ -42490,7 +42748,7 @@
         <v>46028</v>
       </c>
       <c r="M792" t="s">
-        <v>2169</v>
+        <v>7</v>
       </c>
       <c r="N792" t="s">
         <v>8</v>
@@ -42501,7 +42759,7 @@
     </row>
     <row r="793" spans="1:15">
       <c r="A793" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
       <c r="B793" t="s">
         <v>1</v>
@@ -42525,7 +42783,7 @@
         <v>1</v>
       </c>
       <c r="I793" t="s">
-        <v>2215</v>
+        <v>2214</v>
       </c>
       <c r="J793" t="s">
         <v>7</v>
@@ -42535,7 +42793,7 @@
         <v>46028</v>
       </c>
       <c r="M793" t="s">
-        <v>2169</v>
+        <v>7</v>
       </c>
       <c r="N793" t="s">
         <v>8</v>
@@ -42546,7 +42804,7 @@
     </row>
     <row r="794" spans="1:15">
       <c r="A794" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
       <c r="B794" t="s">
         <v>1</v>
@@ -42570,7 +42828,7 @@
         <v>1</v>
       </c>
       <c r="I794" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="J794" t="s">
         <v>7</v>
@@ -42580,7 +42838,7 @@
         <v>46028</v>
       </c>
       <c r="M794" t="s">
-        <v>2169</v>
+        <v>7</v>
       </c>
       <c r="N794" t="s">
         <v>8</v>
@@ -42591,7 +42849,7 @@
     </row>
     <row r="795" spans="1:15">
       <c r="A795" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
       <c r="B795" t="s">
         <v>21</v>
@@ -42615,7 +42873,7 @@
         <v>21</v>
       </c>
       <c r="I795" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="J795" t="s">
         <v>7</v>
@@ -42625,12 +42883,1992 @@
         <v>46028</v>
       </c>
       <c r="M795" t="s">
-        <v>2169</v>
+        <v>7</v>
       </c>
       <c r="N795" t="s">
         <v>8</v>
       </c>
       <c r="O795" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="796" spans="1:15">
+      <c r="A796" t="s">
+        <v>2217</v>
+      </c>
+      <c r="B796" t="s">
+        <v>1</v>
+      </c>
+      <c r="C796" t="s">
+        <v>966</v>
+      </c>
+      <c r="D796" t="s">
+        <v>967</v>
+      </c>
+      <c r="E796" s="2">
+        <v>5</v>
+      </c>
+      <c r="F796" t="s">
+        <v>4</v>
+      </c>
+      <c r="G796" t="s">
+        <v>2218</v>
+      </c>
+      <c r="H796" t="s">
+        <v>1</v>
+      </c>
+      <c r="I796" t="s">
+        <v>293</v>
+      </c>
+      <c r="J796" t="s">
+        <v>7</v>
+      </c>
+      <c r="K796" s="3"/>
+      <c r="L796" s="3">
+        <v>46028</v>
+      </c>
+      <c r="M796" t="s">
+        <v>7</v>
+      </c>
+      <c r="N796" t="s">
+        <v>8</v>
+      </c>
+      <c r="O796" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="797" spans="1:15">
+      <c r="A797" t="s">
+        <v>2219</v>
+      </c>
+      <c r="B797" t="s">
+        <v>53</v>
+      </c>
+      <c r="C797" t="s">
+        <v>881</v>
+      </c>
+      <c r="D797" t="s">
+        <v>882</v>
+      </c>
+      <c r="E797" s="2">
+        <v>50</v>
+      </c>
+      <c r="F797" t="s">
+        <v>4</v>
+      </c>
+      <c r="G797" t="s">
+        <v>1861</v>
+      </c>
+      <c r="H797" t="s">
+        <v>53</v>
+      </c>
+      <c r="I797" t="s">
+        <v>2220</v>
+      </c>
+      <c r="J797" t="s">
+        <v>7</v>
+      </c>
+      <c r="K797" s="3"/>
+      <c r="L797" s="3">
+        <v>46028</v>
+      </c>
+      <c r="M797" t="s">
+        <v>7</v>
+      </c>
+      <c r="N797" t="s">
+        <v>8</v>
+      </c>
+      <c r="O797" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="798" spans="1:15">
+      <c r="A798" t="s">
+        <v>2221</v>
+      </c>
+      <c r="B798" t="s">
+        <v>1</v>
+      </c>
+      <c r="C798" t="s">
+        <v>972</v>
+      </c>
+      <c r="D798" t="s">
+        <v>973</v>
+      </c>
+      <c r="E798" s="2">
+        <v>20</v>
+      </c>
+      <c r="F798" t="s">
+        <v>4</v>
+      </c>
+      <c r="G798" t="s">
+        <v>1974</v>
+      </c>
+      <c r="H798" t="s">
+        <v>1</v>
+      </c>
+      <c r="I798" t="s">
+        <v>2222</v>
+      </c>
+      <c r="J798" t="s">
+        <v>7</v>
+      </c>
+      <c r="K798" s="3"/>
+      <c r="L798" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M798" t="s">
+        <v>7</v>
+      </c>
+      <c r="N798" t="s">
+        <v>8</v>
+      </c>
+      <c r="O798" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="799" spans="1:15">
+      <c r="A799" t="s">
+        <v>2221</v>
+      </c>
+      <c r="B799" t="s">
+        <v>53</v>
+      </c>
+      <c r="C799" t="s">
+        <v>739</v>
+      </c>
+      <c r="D799" t="s">
+        <v>740</v>
+      </c>
+      <c r="E799" s="2">
+        <v>30</v>
+      </c>
+      <c r="F799" t="s">
+        <v>4</v>
+      </c>
+      <c r="G799" t="s">
+        <v>1974</v>
+      </c>
+      <c r="H799" t="s">
+        <v>53</v>
+      </c>
+      <c r="I799" t="s">
+        <v>2222</v>
+      </c>
+      <c r="J799" t="s">
+        <v>7</v>
+      </c>
+      <c r="K799" s="3"/>
+      <c r="L799" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M799" t="s">
+        <v>7</v>
+      </c>
+      <c r="N799" t="s">
+        <v>8</v>
+      </c>
+      <c r="O799" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="800" spans="1:15">
+      <c r="A800" t="s">
+        <v>2223</v>
+      </c>
+      <c r="B800" t="s">
+        <v>1</v>
+      </c>
+      <c r="C800" t="s">
+        <v>743</v>
+      </c>
+      <c r="D800" t="s">
+        <v>744</v>
+      </c>
+      <c r="E800" s="2">
+        <v>60</v>
+      </c>
+      <c r="F800" t="s">
+        <v>4</v>
+      </c>
+      <c r="G800" t="s">
+        <v>1836</v>
+      </c>
+      <c r="H800" t="s">
+        <v>1</v>
+      </c>
+      <c r="I800" t="s">
+        <v>2224</v>
+      </c>
+      <c r="J800" t="s">
+        <v>7</v>
+      </c>
+      <c r="K800" s="3"/>
+      <c r="L800" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M800" t="s">
+        <v>7</v>
+      </c>
+      <c r="N800" t="s">
+        <v>8</v>
+      </c>
+      <c r="O800" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="801" spans="1:15">
+      <c r="A801" t="s">
+        <v>2225</v>
+      </c>
+      <c r="B801" t="s">
+        <v>21</v>
+      </c>
+      <c r="C801" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D801" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E801" s="2">
+        <v>25</v>
+      </c>
+      <c r="F801" t="s">
+        <v>4</v>
+      </c>
+      <c r="G801" t="s">
+        <v>2186</v>
+      </c>
+      <c r="H801" t="s">
+        <v>21</v>
+      </c>
+      <c r="I801" t="s">
+        <v>2226</v>
+      </c>
+      <c r="J801" t="s">
+        <v>7</v>
+      </c>
+      <c r="K801" s="3"/>
+      <c r="L801" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M801" t="s">
+        <v>7</v>
+      </c>
+      <c r="N801" t="s">
+        <v>8</v>
+      </c>
+      <c r="O801" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="802" spans="1:15">
+      <c r="A802" t="s">
+        <v>2227</v>
+      </c>
+      <c r="B802" t="s">
+        <v>25</v>
+      </c>
+      <c r="C802" t="s">
+        <v>907</v>
+      </c>
+      <c r="D802" t="s">
+        <v>908</v>
+      </c>
+      <c r="E802" s="2">
+        <v>125</v>
+      </c>
+      <c r="F802" t="s">
+        <v>4</v>
+      </c>
+      <c r="G802" t="s">
+        <v>1898</v>
+      </c>
+      <c r="H802" t="s">
+        <v>25</v>
+      </c>
+      <c r="I802" t="s">
+        <v>2228</v>
+      </c>
+      <c r="J802" t="s">
+        <v>7</v>
+      </c>
+      <c r="K802" s="3"/>
+      <c r="L802" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M802" t="s">
+        <v>7</v>
+      </c>
+      <c r="N802" t="s">
+        <v>8</v>
+      </c>
+      <c r="O802" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="803" spans="1:15">
+      <c r="A803" t="s">
+        <v>2229</v>
+      </c>
+      <c r="B803" t="s">
+        <v>357</v>
+      </c>
+      <c r="C803" t="s">
+        <v>1245</v>
+      </c>
+      <c r="D803" t="s">
+        <v>55</v>
+      </c>
+      <c r="E803" s="2">
+        <v>25</v>
+      </c>
+      <c r="F803" t="s">
+        <v>4</v>
+      </c>
+      <c r="G803" t="s">
+        <v>1898</v>
+      </c>
+      <c r="H803" t="s">
+        <v>357</v>
+      </c>
+      <c r="I803" t="s">
+        <v>2230</v>
+      </c>
+      <c r="J803" t="s">
+        <v>7</v>
+      </c>
+      <c r="K803" s="3"/>
+      <c r="L803" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M803" t="s">
+        <v>7</v>
+      </c>
+      <c r="N803" t="s">
+        <v>8</v>
+      </c>
+      <c r="O803" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="804" spans="1:15">
+      <c r="A804" t="s">
+        <v>2231</v>
+      </c>
+      <c r="B804" t="s">
+        <v>1</v>
+      </c>
+      <c r="C804" t="s">
+        <v>1050</v>
+      </c>
+      <c r="D804" t="s">
+        <v>1051</v>
+      </c>
+      <c r="E804" s="2">
+        <v>50</v>
+      </c>
+      <c r="F804" t="s">
+        <v>4</v>
+      </c>
+      <c r="G804" t="s">
+        <v>1903</v>
+      </c>
+      <c r="H804" t="s">
+        <v>1</v>
+      </c>
+      <c r="I804" t="s">
+        <v>2232</v>
+      </c>
+      <c r="J804" t="s">
+        <v>7</v>
+      </c>
+      <c r="K804" s="3"/>
+      <c r="L804" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M804" t="s">
+        <v>7</v>
+      </c>
+      <c r="N804" t="s">
+        <v>8</v>
+      </c>
+      <c r="O804" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="805" spans="1:15">
+      <c r="A805" t="s">
+        <v>2233</v>
+      </c>
+      <c r="B805" t="s">
+        <v>21</v>
+      </c>
+      <c r="C805" t="s">
+        <v>1003</v>
+      </c>
+      <c r="D805" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E805" s="2">
+        <v>50</v>
+      </c>
+      <c r="F805" t="s">
+        <v>4</v>
+      </c>
+      <c r="G805" t="s">
+        <v>1861</v>
+      </c>
+      <c r="H805" t="s">
+        <v>21</v>
+      </c>
+      <c r="I805" t="s">
+        <v>2234</v>
+      </c>
+      <c r="J805" t="s">
+        <v>7</v>
+      </c>
+      <c r="K805" s="3"/>
+      <c r="L805" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M805" t="s">
+        <v>7</v>
+      </c>
+      <c r="N805" t="s">
+        <v>8</v>
+      </c>
+      <c r="O805" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="806" spans="1:15">
+      <c r="A806" t="s">
+        <v>2235</v>
+      </c>
+      <c r="B806" t="s">
+        <v>76</v>
+      </c>
+      <c r="C806" t="s">
+        <v>910</v>
+      </c>
+      <c r="D806" t="s">
+        <v>911</v>
+      </c>
+      <c r="E806" s="2">
+        <v>15</v>
+      </c>
+      <c r="F806" t="s">
+        <v>4</v>
+      </c>
+      <c r="G806" t="s">
+        <v>1898</v>
+      </c>
+      <c r="H806" t="s">
+        <v>76</v>
+      </c>
+      <c r="I806" t="s">
+        <v>2236</v>
+      </c>
+      <c r="J806" t="s">
+        <v>7</v>
+      </c>
+      <c r="K806" s="3"/>
+      <c r="L806" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M806" t="s">
+        <v>7</v>
+      </c>
+      <c r="N806" t="s">
+        <v>8</v>
+      </c>
+      <c r="O806" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="807" spans="1:15">
+      <c r="A807" t="s">
+        <v>2235</v>
+      </c>
+      <c r="B807" t="s">
+        <v>82</v>
+      </c>
+      <c r="C807" t="s">
+        <v>1210</v>
+      </c>
+      <c r="D807" t="s">
+        <v>1211</v>
+      </c>
+      <c r="E807" s="2">
+        <v>15</v>
+      </c>
+      <c r="F807" t="s">
+        <v>4</v>
+      </c>
+      <c r="G807" t="s">
+        <v>1898</v>
+      </c>
+      <c r="H807" t="s">
+        <v>82</v>
+      </c>
+      <c r="I807" t="s">
+        <v>2236</v>
+      </c>
+      <c r="J807" t="s">
+        <v>7</v>
+      </c>
+      <c r="K807" s="3"/>
+      <c r="L807" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M807" t="s">
+        <v>7</v>
+      </c>
+      <c r="N807" t="s">
+        <v>8</v>
+      </c>
+      <c r="O807" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="808" spans="1:15">
+      <c r="A808" t="s">
+        <v>2235</v>
+      </c>
+      <c r="B808" t="s">
+        <v>344</v>
+      </c>
+      <c r="C808" t="s">
+        <v>2237</v>
+      </c>
+      <c r="D808" t="s">
+        <v>2238</v>
+      </c>
+      <c r="E808" s="2">
+        <v>25</v>
+      </c>
+      <c r="F808" t="s">
+        <v>4</v>
+      </c>
+      <c r="G808" t="s">
+        <v>1898</v>
+      </c>
+      <c r="H808" t="s">
+        <v>344</v>
+      </c>
+      <c r="I808" t="s">
+        <v>2236</v>
+      </c>
+      <c r="J808" t="s">
+        <v>7</v>
+      </c>
+      <c r="K808" s="3"/>
+      <c r="L808" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M808" t="s">
+        <v>7</v>
+      </c>
+      <c r="N808" t="s">
+        <v>8</v>
+      </c>
+      <c r="O808" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="809" spans="1:15">
+      <c r="A809" t="s">
+        <v>2235</v>
+      </c>
+      <c r="B809" t="s">
+        <v>369</v>
+      </c>
+      <c r="C809" t="s">
+        <v>2239</v>
+      </c>
+      <c r="D809" t="s">
+        <v>2240</v>
+      </c>
+      <c r="E809" s="2">
+        <v>25</v>
+      </c>
+      <c r="F809" t="s">
+        <v>4</v>
+      </c>
+      <c r="G809" t="s">
+        <v>1898</v>
+      </c>
+      <c r="H809" t="s">
+        <v>369</v>
+      </c>
+      <c r="I809" t="s">
+        <v>2236</v>
+      </c>
+      <c r="J809" t="s">
+        <v>7</v>
+      </c>
+      <c r="K809" s="3"/>
+      <c r="L809" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M809" t="s">
+        <v>7</v>
+      </c>
+      <c r="N809" t="s">
+        <v>8</v>
+      </c>
+      <c r="O809" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="810" spans="1:15">
+      <c r="A810" t="s">
+        <v>2241</v>
+      </c>
+      <c r="B810" t="s">
+        <v>73</v>
+      </c>
+      <c r="C810" t="s">
+        <v>1981</v>
+      </c>
+      <c r="D810" t="s">
+        <v>1982</v>
+      </c>
+      <c r="E810" s="2">
+        <v>15</v>
+      </c>
+      <c r="F810" t="s">
+        <v>4</v>
+      </c>
+      <c r="G810" t="s">
+        <v>1898</v>
+      </c>
+      <c r="H810" t="s">
+        <v>73</v>
+      </c>
+      <c r="I810" t="s">
+        <v>2242</v>
+      </c>
+      <c r="J810" t="s">
+        <v>7</v>
+      </c>
+      <c r="K810" s="3"/>
+      <c r="L810" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M810" t="s">
+        <v>7</v>
+      </c>
+      <c r="N810" t="s">
+        <v>8</v>
+      </c>
+      <c r="O810" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="811" spans="1:15">
+      <c r="A811" t="s">
+        <v>2243</v>
+      </c>
+      <c r="B811" t="s">
+        <v>1</v>
+      </c>
+      <c r="C811" t="s">
+        <v>1896</v>
+      </c>
+      <c r="D811" t="s">
+        <v>1897</v>
+      </c>
+      <c r="E811" s="2">
+        <v>80</v>
+      </c>
+      <c r="F811" t="s">
+        <v>4</v>
+      </c>
+      <c r="G811" t="s">
+        <v>1898</v>
+      </c>
+      <c r="H811" t="s">
+        <v>1</v>
+      </c>
+      <c r="I811" t="s">
+        <v>2244</v>
+      </c>
+      <c r="J811" t="s">
+        <v>7</v>
+      </c>
+      <c r="K811" s="3"/>
+      <c r="L811" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M811" t="s">
+        <v>7</v>
+      </c>
+      <c r="N811" t="s">
+        <v>8</v>
+      </c>
+      <c r="O811" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="812" spans="1:15">
+      <c r="A812" t="s">
+        <v>2245</v>
+      </c>
+      <c r="B812" t="s">
+        <v>79</v>
+      </c>
+      <c r="C812" t="s">
+        <v>1232</v>
+      </c>
+      <c r="D812" t="s">
+        <v>1233</v>
+      </c>
+      <c r="E812" s="2">
+        <v>15</v>
+      </c>
+      <c r="F812" t="s">
+        <v>4</v>
+      </c>
+      <c r="G812" t="s">
+        <v>1898</v>
+      </c>
+      <c r="H812" t="s">
+        <v>79</v>
+      </c>
+      <c r="I812" t="s">
+        <v>2246</v>
+      </c>
+      <c r="J812" t="s">
+        <v>7</v>
+      </c>
+      <c r="K812" s="3"/>
+      <c r="L812" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M812" t="s">
+        <v>7</v>
+      </c>
+      <c r="N812" t="s">
+        <v>8</v>
+      </c>
+      <c r="O812" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="813" spans="1:15">
+      <c r="A813" t="s">
+        <v>2247</v>
+      </c>
+      <c r="B813" t="s">
+        <v>1</v>
+      </c>
+      <c r="C813" t="s">
+        <v>1856</v>
+      </c>
+      <c r="D813" t="s">
+        <v>1857</v>
+      </c>
+      <c r="E813" s="2">
+        <v>30</v>
+      </c>
+      <c r="F813" t="s">
+        <v>4</v>
+      </c>
+      <c r="G813" t="s">
+        <v>1858</v>
+      </c>
+      <c r="H813" t="s">
+        <v>1</v>
+      </c>
+      <c r="I813" t="s">
+        <v>1859</v>
+      </c>
+      <c r="J813" t="s">
+        <v>7</v>
+      </c>
+      <c r="K813" s="3"/>
+      <c r="L813" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M813" t="s">
+        <v>7</v>
+      </c>
+      <c r="N813" t="s">
+        <v>8</v>
+      </c>
+      <c r="O813" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="814" spans="1:15">
+      <c r="A814" t="s">
+        <v>2248</v>
+      </c>
+      <c r="B814" t="s">
+        <v>53</v>
+      </c>
+      <c r="C814" t="s">
+        <v>751</v>
+      </c>
+      <c r="D814" t="s">
+        <v>752</v>
+      </c>
+      <c r="E814" s="2">
+        <v>15</v>
+      </c>
+      <c r="F814" t="s">
+        <v>4</v>
+      </c>
+      <c r="G814" t="s">
+        <v>1994</v>
+      </c>
+      <c r="H814" t="s">
+        <v>53</v>
+      </c>
+      <c r="I814" t="s">
+        <v>2249</v>
+      </c>
+      <c r="J814" t="s">
+        <v>7</v>
+      </c>
+      <c r="K814" s="3"/>
+      <c r="L814" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M814" t="s">
+        <v>7</v>
+      </c>
+      <c r="N814" t="s">
+        <v>8</v>
+      </c>
+      <c r="O814" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="815" spans="1:15">
+      <c r="A815" t="s">
+        <v>2248</v>
+      </c>
+      <c r="B815" t="s">
+        <v>21</v>
+      </c>
+      <c r="C815" t="s">
+        <v>2250</v>
+      </c>
+      <c r="D815" t="s">
+        <v>2251</v>
+      </c>
+      <c r="E815" s="2">
+        <v>15</v>
+      </c>
+      <c r="F815" t="s">
+        <v>4</v>
+      </c>
+      <c r="G815" t="s">
+        <v>1994</v>
+      </c>
+      <c r="H815" t="s">
+        <v>21</v>
+      </c>
+      <c r="I815" t="s">
+        <v>2249</v>
+      </c>
+      <c r="J815" t="s">
+        <v>7</v>
+      </c>
+      <c r="K815" s="3"/>
+      <c r="L815" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M815" t="s">
+        <v>7</v>
+      </c>
+      <c r="N815" t="s">
+        <v>8</v>
+      </c>
+      <c r="O815" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="816" spans="1:15">
+      <c r="A816" t="s">
+        <v>2248</v>
+      </c>
+      <c r="B816" t="s">
+        <v>25</v>
+      </c>
+      <c r="C816" t="s">
+        <v>745</v>
+      </c>
+      <c r="D816" t="s">
+        <v>746</v>
+      </c>
+      <c r="E816" s="2">
+        <v>15</v>
+      </c>
+      <c r="F816" t="s">
+        <v>4</v>
+      </c>
+      <c r="G816" t="s">
+        <v>1994</v>
+      </c>
+      <c r="H816" t="s">
+        <v>25</v>
+      </c>
+      <c r="I816" t="s">
+        <v>2249</v>
+      </c>
+      <c r="J816" t="s">
+        <v>7</v>
+      </c>
+      <c r="K816" s="3"/>
+      <c r="L816" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M816" t="s">
+        <v>7</v>
+      </c>
+      <c r="N816" t="s">
+        <v>8</v>
+      </c>
+      <c r="O816" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="817" spans="1:15">
+      <c r="A817" t="s">
+        <v>2248</v>
+      </c>
+      <c r="B817" t="s">
+        <v>73</v>
+      </c>
+      <c r="C817" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D817" t="s">
+        <v>1123</v>
+      </c>
+      <c r="E817" s="2">
+        <v>15</v>
+      </c>
+      <c r="F817" t="s">
+        <v>4</v>
+      </c>
+      <c r="G817" t="s">
+        <v>1994</v>
+      </c>
+      <c r="H817" t="s">
+        <v>73</v>
+      </c>
+      <c r="I817" t="s">
+        <v>2249</v>
+      </c>
+      <c r="J817" t="s">
+        <v>7</v>
+      </c>
+      <c r="K817" s="3"/>
+      <c r="L817" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M817" t="s">
+        <v>7</v>
+      </c>
+      <c r="N817" t="s">
+        <v>8</v>
+      </c>
+      <c r="O817" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="818" spans="1:15">
+      <c r="A818" t="s">
+        <v>2252</v>
+      </c>
+      <c r="B818" t="s">
+        <v>21</v>
+      </c>
+      <c r="C818" t="s">
+        <v>704</v>
+      </c>
+      <c r="D818" t="s">
+        <v>55</v>
+      </c>
+      <c r="E818" s="2">
+        <v>134</v>
+      </c>
+      <c r="F818" t="s">
+        <v>4</v>
+      </c>
+      <c r="G818" t="s">
+        <v>1898</v>
+      </c>
+      <c r="H818" t="s">
+        <v>21</v>
+      </c>
+      <c r="I818" t="s">
+        <v>2253</v>
+      </c>
+      <c r="J818" t="s">
+        <v>7</v>
+      </c>
+      <c r="K818" s="3"/>
+      <c r="L818" s="3">
+        <v>46029</v>
+      </c>
+      <c r="M818" t="s">
+        <v>7</v>
+      </c>
+      <c r="N818" t="s">
+        <v>8</v>
+      </c>
+      <c r="O818" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="819" spans="1:15">
+      <c r="A819" t="s">
+        <v>2254</v>
+      </c>
+      <c r="B819" t="s">
+        <v>1</v>
+      </c>
+      <c r="C819" t="s">
+        <v>2255</v>
+      </c>
+      <c r="D819" t="s">
+        <v>2256</v>
+      </c>
+      <c r="E819" s="2">
+        <v>20</v>
+      </c>
+      <c r="F819" t="s">
+        <v>4</v>
+      </c>
+      <c r="G819" t="s">
+        <v>2257</v>
+      </c>
+      <c r="H819" t="s">
+        <v>1</v>
+      </c>
+      <c r="I819" t="s">
+        <v>2258</v>
+      </c>
+      <c r="J819" t="s">
+        <v>7</v>
+      </c>
+      <c r="K819" s="3"/>
+      <c r="L819" s="3">
+        <v>46030</v>
+      </c>
+      <c r="M819" t="s">
+        <v>7</v>
+      </c>
+      <c r="N819" t="s">
+        <v>8</v>
+      </c>
+      <c r="O819" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="820" spans="1:15">
+      <c r="A820" t="s">
+        <v>2259</v>
+      </c>
+      <c r="B820" t="s">
+        <v>1</v>
+      </c>
+      <c r="C820" t="s">
+        <v>2260</v>
+      </c>
+      <c r="D820" t="s">
+        <v>2261</v>
+      </c>
+      <c r="E820" s="2">
+        <v>5</v>
+      </c>
+      <c r="F820" t="s">
+        <v>4</v>
+      </c>
+      <c r="G820" t="s">
+        <v>2262</v>
+      </c>
+      <c r="H820" t="s">
+        <v>1</v>
+      </c>
+      <c r="I820" t="s">
+        <v>2263</v>
+      </c>
+      <c r="J820" t="s">
+        <v>7</v>
+      </c>
+      <c r="K820" s="3"/>
+      <c r="L820" s="3">
+        <v>46034</v>
+      </c>
+      <c r="M820" t="s">
+        <v>7</v>
+      </c>
+      <c r="N820" t="s">
+        <v>8</v>
+      </c>
+      <c r="O820" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="821" spans="1:15">
+      <c r="A821" t="s">
+        <v>2264</v>
+      </c>
+      <c r="B821" t="s">
+        <v>53</v>
+      </c>
+      <c r="C821" t="s">
+        <v>1912</v>
+      </c>
+      <c r="D821" t="s">
+        <v>1913</v>
+      </c>
+      <c r="E821" s="2">
+        <v>30</v>
+      </c>
+      <c r="F821" t="s">
+        <v>4</v>
+      </c>
+      <c r="G821" t="s">
+        <v>2014</v>
+      </c>
+      <c r="H821" t="s">
+        <v>53</v>
+      </c>
+      <c r="I821" t="s">
+        <v>2265</v>
+      </c>
+      <c r="J821" t="s">
+        <v>7</v>
+      </c>
+      <c r="K821" s="3"/>
+      <c r="L821" s="3">
+        <v>46034</v>
+      </c>
+      <c r="M821" t="s">
+        <v>7</v>
+      </c>
+      <c r="N821" t="s">
+        <v>8</v>
+      </c>
+      <c r="O821" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="822" spans="1:15">
+      <c r="A822" t="s">
+        <v>2264</v>
+      </c>
+      <c r="B822" t="s">
+        <v>82</v>
+      </c>
+      <c r="C822" t="s">
+        <v>2266</v>
+      </c>
+      <c r="D822" t="s">
+        <v>2267</v>
+      </c>
+      <c r="E822" s="2">
+        <v>25</v>
+      </c>
+      <c r="F822" t="s">
+        <v>4</v>
+      </c>
+      <c r="G822" t="s">
+        <v>2014</v>
+      </c>
+      <c r="H822" t="s">
+        <v>82</v>
+      </c>
+      <c r="I822" t="s">
+        <v>2265</v>
+      </c>
+      <c r="J822" t="s">
+        <v>7</v>
+      </c>
+      <c r="K822" s="3"/>
+      <c r="L822" s="3">
+        <v>46034</v>
+      </c>
+      <c r="M822" t="s">
+        <v>7</v>
+      </c>
+      <c r="N822" t="s">
+        <v>8</v>
+      </c>
+      <c r="O822" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="823" spans="1:15">
+      <c r="A823" t="s">
+        <v>2268</v>
+      </c>
+      <c r="B823" t="s">
+        <v>1</v>
+      </c>
+      <c r="C823" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D823" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E823" s="2">
+        <v>15</v>
+      </c>
+      <c r="F823" t="s">
+        <v>4</v>
+      </c>
+      <c r="G823" t="s">
+        <v>1994</v>
+      </c>
+      <c r="H823" t="s">
+        <v>1</v>
+      </c>
+      <c r="I823" t="s">
+        <v>2249</v>
+      </c>
+      <c r="J823" t="s">
+        <v>7</v>
+      </c>
+      <c r="K823" s="3"/>
+      <c r="L823" s="3">
+        <v>46034</v>
+      </c>
+      <c r="M823" t="s">
+        <v>7</v>
+      </c>
+      <c r="N823" t="s">
+        <v>8</v>
+      </c>
+      <c r="O823" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="824" spans="1:15">
+      <c r="A824" t="s">
+        <v>2269</v>
+      </c>
+      <c r="B824" t="s">
+        <v>1</v>
+      </c>
+      <c r="C824" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D824" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E824" s="2">
+        <v>50</v>
+      </c>
+      <c r="F824" t="s">
+        <v>4</v>
+      </c>
+      <c r="G824" t="s">
+        <v>1861</v>
+      </c>
+      <c r="H824" t="s">
+        <v>1</v>
+      </c>
+      <c r="I824" t="s">
+        <v>2270</v>
+      </c>
+      <c r="J824" t="s">
+        <v>7</v>
+      </c>
+      <c r="K824" s="3"/>
+      <c r="L824" s="3">
+        <v>46035</v>
+      </c>
+      <c r="M824" t="s">
+        <v>7</v>
+      </c>
+      <c r="N824" t="s">
+        <v>8</v>
+      </c>
+      <c r="O824" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="825" spans="1:15">
+      <c r="A825" t="s">
+        <v>2271</v>
+      </c>
+      <c r="B825" t="s">
+        <v>1</v>
+      </c>
+      <c r="C825" t="s">
+        <v>825</v>
+      </c>
+      <c r="D825" t="s">
+        <v>826</v>
+      </c>
+      <c r="E825" s="2">
+        <v>15</v>
+      </c>
+      <c r="F825" t="s">
+        <v>4</v>
+      </c>
+      <c r="G825" t="s">
+        <v>2272</v>
+      </c>
+      <c r="H825" t="s">
+        <v>1</v>
+      </c>
+      <c r="I825" t="s">
+        <v>2273</v>
+      </c>
+      <c r="J825" t="s">
+        <v>7</v>
+      </c>
+      <c r="K825" s="3"/>
+      <c r="L825" s="3">
+        <v>46037</v>
+      </c>
+      <c r="M825" t="s">
+        <v>7</v>
+      </c>
+      <c r="N825" t="s">
+        <v>8</v>
+      </c>
+      <c r="O825" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="826" spans="1:15">
+      <c r="A826" t="s">
+        <v>2274</v>
+      </c>
+      <c r="B826" t="s">
+        <v>21</v>
+      </c>
+      <c r="C826" t="s">
+        <v>704</v>
+      </c>
+      <c r="D826" t="s">
+        <v>55</v>
+      </c>
+      <c r="E826" s="2">
+        <v>1</v>
+      </c>
+      <c r="F826" t="s">
+        <v>4</v>
+      </c>
+      <c r="G826" t="s">
+        <v>1898</v>
+      </c>
+      <c r="H826" t="s">
+        <v>21</v>
+      </c>
+      <c r="I826" t="s">
+        <v>2275</v>
+      </c>
+      <c r="J826" t="s">
+        <v>7</v>
+      </c>
+      <c r="K826" s="3"/>
+      <c r="L826" s="3">
+        <v>46037</v>
+      </c>
+      <c r="M826" t="s">
+        <v>7</v>
+      </c>
+      <c r="N826" t="s">
+        <v>8</v>
+      </c>
+      <c r="O826" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="827" spans="1:15">
+      <c r="A827" t="s">
+        <v>2276</v>
+      </c>
+      <c r="B827" t="s">
+        <v>53</v>
+      </c>
+      <c r="C827" t="s">
+        <v>54</v>
+      </c>
+      <c r="D827" t="s">
+        <v>55</v>
+      </c>
+      <c r="E827" s="2">
+        <v>10</v>
+      </c>
+      <c r="F827" t="s">
+        <v>4</v>
+      </c>
+      <c r="G827" t="s">
+        <v>2272</v>
+      </c>
+      <c r="H827" t="s">
+        <v>53</v>
+      </c>
+      <c r="I827" t="s">
+        <v>2277</v>
+      </c>
+      <c r="J827" t="s">
+        <v>7</v>
+      </c>
+      <c r="K827" s="3"/>
+      <c r="L827" s="3">
+        <v>46037</v>
+      </c>
+      <c r="M827" t="s">
+        <v>7</v>
+      </c>
+      <c r="N827" t="s">
+        <v>8</v>
+      </c>
+      <c r="O827" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="828" spans="1:15">
+      <c r="A828" t="s">
+        <v>2278</v>
+      </c>
+      <c r="B828" t="s">
+        <v>1</v>
+      </c>
+      <c r="C828" t="s">
+        <v>290</v>
+      </c>
+      <c r="D828" t="s">
+        <v>291</v>
+      </c>
+      <c r="E828" s="2">
+        <v>62</v>
+      </c>
+      <c r="F828" t="s">
+        <v>4</v>
+      </c>
+      <c r="G828" t="s">
+        <v>2279</v>
+      </c>
+      <c r="H828" t="s">
+        <v>1</v>
+      </c>
+      <c r="I828" t="s">
+        <v>2280</v>
+      </c>
+      <c r="J828" t="s">
+        <v>7</v>
+      </c>
+      <c r="K828" s="3"/>
+      <c r="L828" s="3">
+        <v>46037</v>
+      </c>
+      <c r="M828" t="s">
+        <v>7</v>
+      </c>
+      <c r="N828" t="s">
+        <v>8</v>
+      </c>
+      <c r="O828" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="829" spans="1:15">
+      <c r="A829" t="s">
+        <v>2281</v>
+      </c>
+      <c r="B829" t="s">
+        <v>21</v>
+      </c>
+      <c r="C829" t="s">
+        <v>1133</v>
+      </c>
+      <c r="D829" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E829" s="2">
+        <v>25</v>
+      </c>
+      <c r="F829" t="s">
+        <v>4</v>
+      </c>
+      <c r="G829" t="s">
+        <v>2282</v>
+      </c>
+      <c r="H829" t="s">
+        <v>21</v>
+      </c>
+      <c r="I829" t="s">
+        <v>2283</v>
+      </c>
+      <c r="J829" t="s">
+        <v>7</v>
+      </c>
+      <c r="K829" s="3"/>
+      <c r="L829" s="3">
+        <v>46037</v>
+      </c>
+      <c r="M829" t="s">
+        <v>7</v>
+      </c>
+      <c r="N829" t="s">
+        <v>8</v>
+      </c>
+      <c r="O829" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="830" spans="1:15">
+      <c r="A830" t="s">
+        <v>2284</v>
+      </c>
+      <c r="B830" t="s">
+        <v>53</v>
+      </c>
+      <c r="C830" t="s">
+        <v>16</v>
+      </c>
+      <c r="D830" t="s">
+        <v>17</v>
+      </c>
+      <c r="E830" s="2">
+        <v>25</v>
+      </c>
+      <c r="F830" t="s">
+        <v>4</v>
+      </c>
+      <c r="G830" t="s">
+        <v>2282</v>
+      </c>
+      <c r="H830" t="s">
+        <v>53</v>
+      </c>
+      <c r="I830" t="s">
+        <v>2285</v>
+      </c>
+      <c r="J830" t="s">
+        <v>7</v>
+      </c>
+      <c r="K830" s="3"/>
+      <c r="L830" s="3">
+        <v>46037</v>
+      </c>
+      <c r="M830" t="s">
+        <v>7</v>
+      </c>
+      <c r="N830" t="s">
+        <v>8</v>
+      </c>
+      <c r="O830" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="831" spans="1:15">
+      <c r="A831" t="s">
+        <v>2286</v>
+      </c>
+      <c r="B831" t="s">
+        <v>25</v>
+      </c>
+      <c r="C831" t="s">
+        <v>2287</v>
+      </c>
+      <c r="D831" t="s">
+        <v>2288</v>
+      </c>
+      <c r="E831" s="2">
+        <v>25</v>
+      </c>
+      <c r="F831" t="s">
+        <v>4</v>
+      </c>
+      <c r="G831" t="s">
+        <v>2282</v>
+      </c>
+      <c r="H831" t="s">
+        <v>25</v>
+      </c>
+      <c r="I831" t="s">
+        <v>2289</v>
+      </c>
+      <c r="J831" t="s">
+        <v>7</v>
+      </c>
+      <c r="K831" s="3"/>
+      <c r="L831" s="3">
+        <v>46042</v>
+      </c>
+      <c r="M831" t="s">
+        <v>7</v>
+      </c>
+      <c r="N831" t="s">
+        <v>8</v>
+      </c>
+      <c r="O831" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="832" spans="1:15">
+      <c r="A832" t="s">
+        <v>2290</v>
+      </c>
+      <c r="B832" t="s">
+        <v>1</v>
+      </c>
+      <c r="C832" t="s">
+        <v>424</v>
+      </c>
+      <c r="D832" t="s">
+        <v>425</v>
+      </c>
+      <c r="E832" s="2">
+        <v>600</v>
+      </c>
+      <c r="F832" t="s">
+        <v>4</v>
+      </c>
+      <c r="G832" t="s">
+        <v>2291</v>
+      </c>
+      <c r="H832" t="s">
+        <v>1</v>
+      </c>
+      <c r="I832" t="s">
+        <v>2292</v>
+      </c>
+      <c r="J832" t="s">
+        <v>7</v>
+      </c>
+      <c r="K832" s="3"/>
+      <c r="L832" s="3">
+        <v>46042</v>
+      </c>
+      <c r="M832" t="s">
+        <v>7</v>
+      </c>
+      <c r="N832" t="s">
+        <v>8</v>
+      </c>
+      <c r="O832" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="833" spans="1:15">
+      <c r="A833" t="s">
+        <v>2293</v>
+      </c>
+      <c r="B833" t="s">
+        <v>1</v>
+      </c>
+      <c r="C833" t="s">
+        <v>724</v>
+      </c>
+      <c r="D833" t="s">
+        <v>725</v>
+      </c>
+      <c r="E833" s="2">
+        <v>2</v>
+      </c>
+      <c r="F833" t="s">
+        <v>4</v>
+      </c>
+      <c r="G833" t="s">
+        <v>2294</v>
+      </c>
+      <c r="H833" t="s">
+        <v>1</v>
+      </c>
+      <c r="I833" t="s">
+        <v>2295</v>
+      </c>
+      <c r="J833" t="s">
+        <v>7</v>
+      </c>
+      <c r="K833" s="3"/>
+      <c r="L833" s="3">
+        <v>46042</v>
+      </c>
+      <c r="M833" t="s">
+        <v>7</v>
+      </c>
+      <c r="N833" t="s">
+        <v>8</v>
+      </c>
+      <c r="O833" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="834" spans="1:15">
+      <c r="A834" t="s">
+        <v>2296</v>
+      </c>
+      <c r="B834" t="s">
+        <v>1</v>
+      </c>
+      <c r="C834" t="s">
+        <v>592</v>
+      </c>
+      <c r="D834" t="s">
+        <v>593</v>
+      </c>
+      <c r="E834" s="2">
+        <v>100</v>
+      </c>
+      <c r="F834" t="s">
+        <v>4</v>
+      </c>
+      <c r="G834" t="s">
+        <v>2297</v>
+      </c>
+      <c r="H834" t="s">
+        <v>1</v>
+      </c>
+      <c r="I834" t="s">
+        <v>293</v>
+      </c>
+      <c r="J834" t="s">
+        <v>7</v>
+      </c>
+      <c r="K834" s="3"/>
+      <c r="L834" s="3">
+        <v>46043</v>
+      </c>
+      <c r="M834" t="s">
+        <v>7</v>
+      </c>
+      <c r="N834" t="s">
+        <v>8</v>
+      </c>
+      <c r="O834" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="835" spans="1:15">
+      <c r="A835" t="s">
+        <v>2298</v>
+      </c>
+      <c r="B835" t="s">
+        <v>1</v>
+      </c>
+      <c r="C835" t="s">
+        <v>1705</v>
+      </c>
+      <c r="D835" t="s">
+        <v>1706</v>
+      </c>
+      <c r="E835" s="2">
+        <v>50</v>
+      </c>
+      <c r="F835" t="s">
+        <v>4</v>
+      </c>
+      <c r="G835" t="s">
+        <v>2299</v>
+      </c>
+      <c r="H835" t="s">
+        <v>1</v>
+      </c>
+      <c r="I835" t="s">
+        <v>2300</v>
+      </c>
+      <c r="J835" t="s">
+        <v>7</v>
+      </c>
+      <c r="K835" s="3"/>
+      <c r="L835" s="3">
+        <v>46044</v>
+      </c>
+      <c r="M835" t="s">
+        <v>7</v>
+      </c>
+      <c r="N835" t="s">
+        <v>8</v>
+      </c>
+      <c r="O835" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="836" spans="1:15">
+      <c r="A836" t="s">
+        <v>2301</v>
+      </c>
+      <c r="B836" t="s">
+        <v>1</v>
+      </c>
+      <c r="C836" t="s">
+        <v>2176</v>
+      </c>
+      <c r="D836" t="s">
+        <v>2177</v>
+      </c>
+      <c r="E836" s="2">
+        <v>6</v>
+      </c>
+      <c r="F836" t="s">
+        <v>4</v>
+      </c>
+      <c r="G836" t="s">
+        <v>2178</v>
+      </c>
+      <c r="H836" t="s">
+        <v>1</v>
+      </c>
+      <c r="I836" t="s">
+        <v>2179</v>
+      </c>
+      <c r="J836" t="s">
+        <v>7</v>
+      </c>
+      <c r="K836" s="3"/>
+      <c r="L836" s="3">
+        <v>46044</v>
+      </c>
+      <c r="M836" t="s">
+        <v>7</v>
+      </c>
+      <c r="N836" t="s">
+        <v>8</v>
+      </c>
+      <c r="O836" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="837" spans="1:15">
+      <c r="A837" t="s">
+        <v>2301</v>
+      </c>
+      <c r="B837" t="s">
+        <v>53</v>
+      </c>
+      <c r="C837" t="s">
+        <v>2181</v>
+      </c>
+      <c r="D837" t="s">
+        <v>2182</v>
+      </c>
+      <c r="E837" s="2">
+        <v>6</v>
+      </c>
+      <c r="F837" t="s">
+        <v>4</v>
+      </c>
+      <c r="G837" t="s">
+        <v>2178</v>
+      </c>
+      <c r="H837" t="s">
+        <v>53</v>
+      </c>
+      <c r="I837" t="s">
+        <v>2179</v>
+      </c>
+      <c r="J837" t="s">
+        <v>7</v>
+      </c>
+      <c r="K837" s="3"/>
+      <c r="L837" s="3">
+        <v>46044</v>
+      </c>
+      <c r="M837" t="s">
+        <v>7</v>
+      </c>
+      <c r="N837" t="s">
+        <v>8</v>
+      </c>
+      <c r="O837" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="838" spans="1:15">
+      <c r="A838" t="s">
+        <v>2301</v>
+      </c>
+      <c r="B838" t="s">
+        <v>21</v>
+      </c>
+      <c r="C838" t="s">
+        <v>2183</v>
+      </c>
+      <c r="D838" t="s">
+        <v>2184</v>
+      </c>
+      <c r="E838" s="2">
+        <v>8</v>
+      </c>
+      <c r="F838" t="s">
+        <v>4</v>
+      </c>
+      <c r="G838" t="s">
+        <v>2178</v>
+      </c>
+      <c r="H838" t="s">
+        <v>21</v>
+      </c>
+      <c r="I838" t="s">
+        <v>2179</v>
+      </c>
+      <c r="J838" t="s">
+        <v>7</v>
+      </c>
+      <c r="K838" s="3"/>
+      <c r="L838" s="3">
+        <v>46044</v>
+      </c>
+      <c r="M838" t="s">
+        <v>7</v>
+      </c>
+      <c r="N838" t="s">
+        <v>8</v>
+      </c>
+      <c r="O838" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="839" spans="1:15">
+      <c r="A839" t="s">
+        <v>2302</v>
+      </c>
+      <c r="B839" t="s">
+        <v>1</v>
+      </c>
+      <c r="C839" t="s">
+        <v>2072</v>
+      </c>
+      <c r="D839" t="s">
+        <v>2073</v>
+      </c>
+      <c r="E839" s="2">
+        <v>25</v>
+      </c>
+      <c r="F839" t="s">
+        <v>4</v>
+      </c>
+      <c r="G839" t="s">
+        <v>2074</v>
+      </c>
+      <c r="H839" t="s">
+        <v>1</v>
+      </c>
+      <c r="I839" t="s">
+        <v>2303</v>
+      </c>
+      <c r="J839" t="s">
+        <v>7</v>
+      </c>
+      <c r="K839" s="3"/>
+      <c r="L839" s="3">
+        <v>46048</v>
+      </c>
+      <c r="M839" t="s">
+        <v>7</v>
+      </c>
+      <c r="N839" t="s">
+        <v>8</v>
+      </c>
+      <c r="O839" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>